<commit_message>
Creating generalized launch_intent prompt type.
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108" count="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="123" count="171">
   <si>
     <t>type</t>
   </si>
@@ -34,6 +34,9 @@
     <t>hint</t>
   </si>
   <si>
+    <t>default</t>
+  </si>
+  <si>
     <t>audio</t>
   </si>
   <si>
@@ -64,6 +67,39 @@
     <t>Which examples would you like to see?</t>
   </si>
   <si>
+    <t>goto intents_end</t>
+  </si>
+  <si>
+    <t>not(selected(data('examples'), 'intents'))</t>
+  </si>
+  <si>
+    <t>barcode</t>
+  </si>
+  <si>
+    <t>Scan a barcode</t>
+  </si>
+  <si>
+    <t>pulseox</t>
+  </si>
+  <si>
+    <t>Record blood oxygen level</t>
+  </si>
+  <si>
+    <t>picture</t>
+  </si>
+  <si>
+    <t>Take a picture</t>
+  </si>
+  <si>
+    <t>recording</t>
+  </si>
+  <si>
+    <t>Make a recording</t>
+  </si>
+  <si>
+    <t>label intents_end</t>
+  </si>
+  <si>
     <t>goto dynamic_label_end</t>
   </si>
   <si>
@@ -103,6 +139,12 @@
     <t>When were you born?</t>
   </si>
   <si>
+    <t>data('born').getDay() === now().getDay() &amp;&amp; data('born').getMonth() === now().getMonth()</t>
+  </si>
+  <si>
+    <t>Happy Birthday!</t>
+  </si>
+  <si>
     <t>time</t>
   </si>
   <si>
@@ -293,6 +335,9 @@
   </si>
   <si>
     <t>Antarctica</t>
+  </si>
+  <si>
+    <t>intents</t>
   </si>
   <si>
     <t>dynamic_label</t>
@@ -452,13 +497,13 @@
     <col max="4" min="4" customWidth="1" width="19.14"/>
     <col max="5" min="5" customWidth="1" width="41.86"/>
     <col max="6" min="6" customWidth="1" width="40.0"/>
-    <col max="7" min="7" customWidth="1" width="20.57"/>
-    <col max="8" min="8" customWidth="1" width="13.0"/>
-    <col max="9" min="9" customWidth="1" width="15.86"/>
-    <col max="10" min="10" customWidth="1" width="18.29"/>
-    <col max="11" min="11" customWidth="1" width="18.43"/>
-    <col max="12" min="12" customWidth="1" width="19.0"/>
-    <col max="13" min="13" customWidth="1" width="27.0"/>
+    <col max="8" min="8" customWidth="1" width="20.57"/>
+    <col max="9" min="9" customWidth="1" width="13.0"/>
+    <col max="10" min="10" customWidth="1" width="15.86"/>
+    <col max="11" min="11" customWidth="1" width="18.29"/>
+    <col max="12" min="12" customWidth="1" width="18.43"/>
+    <col max="13" min="13" customWidth="1" width="19.0"/>
+    <col max="14" min="14" customWidth="1" width="27.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -501,168 +546,177 @@
       <c t="s" s="1" r="M1">
         <v>12</v>
       </c>
+      <c t="s" s="1" r="N1">
+        <v>13</v>
+      </c>
     </row>
     <row ht="18.0" r="2" customHeight="1">
       <c t="s" s="1" r="A2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c t="s" r="C2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c t="s" r="E2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="2" r="A3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
-      <c t="s" s="1" r="A4">
-        <v>18</v>
-      </c>
-      <c t="s" s="1" r="C4">
-        <v>2</v>
-      </c>
-      <c t="s" s="1" r="E4">
+      <c t="s" r="A4">
         <v>19</v>
       </c>
-      <c t="s" s="1" r="F4">
+      <c t="s" r="C4">
+        <v>19</v>
+      </c>
+      <c t="s" r="E4">
         <v>20</v>
       </c>
     </row>
     <row r="5">
-      <c t="s" s="1" r="A5">
+      <c t="s" r="A5">
         <v>21</v>
       </c>
-      <c t="s" s="1" r="E5">
+      <c t="s" r="C5">
+        <v>21</v>
+      </c>
+      <c t="s" r="E5">
         <v>22</v>
       </c>
     </row>
-    <row ht="18.0" r="6" customHeight="1">
-      <c t="s" s="3" r="A6">
+    <row r="6">
+      <c t="s" r="A6">
+        <v>8</v>
+      </c>
+      <c t="s" r="C6">
         <v>23</v>
       </c>
-    </row>
-    <row ht="18.0" r="7" customHeight="1">
-      <c t="s" s="2" r="A7">
+      <c t="s" r="E6">
         <v>24</v>
       </c>
-      <c t="s" s="1" r="B7">
+    </row>
+    <row r="7">
+      <c t="s" r="A7">
+        <v>7</v>
+      </c>
+      <c t="s" r="C7">
         <v>25</v>
       </c>
-    </row>
-    <row ht="18.0" r="8" customHeight="1">
-      <c t="s" s="1" r="A8">
+      <c t="s" r="E7">
         <v>26</v>
       </c>
-      <c t="s" r="C8">
+    </row>
+    <row r="8">
+      <c t="s" s="3" r="A8">
         <v>27</v>
       </c>
-      <c t="s" s="1" r="E8">
+    </row>
+    <row r="9">
+      <c t="s" s="2" r="A9">
         <v>28</v>
       </c>
-    </row>
-    <row ht="18.0" r="9" customHeight="1">
-      <c t="s" s="1" r="A9">
+      <c t="s" s="1" r="B9">
         <v>29</v>
-      </c>
-      <c t="s" r="C9">
-        <v>29</v>
-      </c>
-      <c t="s" s="1" r="E9">
-        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
+        <v>30</v>
+      </c>
+      <c t="s" s="1" r="C10">
+        <v>2</v>
+      </c>
+      <c t="s" s="1" r="E10">
         <v>31</v>
       </c>
-      <c t="s" s="1" r="C10">
-        <v>31</v>
-      </c>
-      <c t="s" s="1" r="E10">
+      <c t="s" s="1" r="F10">
         <v>32</v>
       </c>
     </row>
-    <row ht="18.0" r="11" customHeight="1">
-      <c t="s" s="3" r="A11">
+    <row r="11">
+      <c t="s" s="1" r="A11">
         <v>33</v>
       </c>
-      <c s="1" r="C11"/>
+      <c t="s" s="1" r="E11">
+        <v>34</v>
+      </c>
     </row>
     <row ht="18.0" r="12" customHeight="1">
-      <c t="s" s="1" r="A12">
-        <v>34</v>
-      </c>
-      <c t="s" r="B12">
+      <c t="s" s="3" r="A12">
         <v>35</v>
       </c>
-      <c t="s" s="1" r="C12">
+    </row>
+    <row ht="18.0" r="13" customHeight="1">
+      <c t="s" s="2" r="A13">
         <v>36</v>
       </c>
-      <c t="s" s="1" r="E12">
+      <c t="s" s="1" r="B13">
         <v>37</v>
       </c>
     </row>
-    <row r="13">
-      <c t="s" s="1" r="A13">
+    <row ht="18.0" r="14" customHeight="1">
+      <c t="s" s="1" r="A14">
         <v>38</v>
       </c>
-      <c t="s" r="B13">
+      <c t="s" r="C14">
         <v>39</v>
       </c>
-    </row>
-    <row r="14">
-      <c t="s" s="1" r="A14">
+      <c t="s" s="1" r="E14">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="C14">
+    </row>
+    <row ht="18.0" r="15" customHeight="1">
+      <c t="s" s="1" r="A15">
+        <v>33</v>
+      </c>
+      <c t="s" r="C15">
         <v>41</v>
       </c>
-      <c t="s" s="1" r="E14">
+      <c t="s" s="1" r="E15">
         <v>42</v>
       </c>
     </row>
-    <row r="15">
-      <c t="s" s="1" r="A15">
+    <row ht="18.0" r="16" customHeight="1">
+      <c t="s" s="1" r="A16">
         <v>43</v>
       </c>
-      <c t="s" s="1" r="B15">
+      <c t="s" r="C16">
+        <v>43</v>
+      </c>
+      <c t="s" s="1" r="E16">
         <v>44</v>
       </c>
-      <c t="s" s="1" r="C15">
+    </row>
+    <row r="17">
+      <c t="s" s="1" r="A17">
         <v>45</v>
       </c>
-      <c t="s" s="1" r="E15">
+      <c t="s" s="1" r="C17">
+        <v>45</v>
+      </c>
+      <c t="s" s="1" r="E17">
         <v>46</v>
       </c>
     </row>
-    <row r="16">
-      <c t="s" s="1" r="A16">
+    <row ht="18.0" r="18" customHeight="1">
+      <c t="s" s="3" r="A18">
         <v>47</v>
       </c>
-    </row>
-    <row r="17">
-      <c t="s" s="4" r="A17">
+      <c s="1" r="C18"/>
+    </row>
+    <row ht="18.0" r="19" customHeight="1">
+      <c t="s" s="1" r="A19">
         <v>48</v>
       </c>
-      <c t="s" r="B17">
+      <c t="s" r="B19">
         <v>49</v>
-      </c>
-    </row>
-    <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19">
-      <c t="s" s="1" r="A19">
-        <v>6</v>
       </c>
       <c t="s" s="1" r="C19">
         <v>50</v>
@@ -675,16 +729,13 @@
       <c t="s" s="1" r="A20">
         <v>52</v>
       </c>
-      <c t="s" s="1" r="C20">
+      <c t="s" r="B20">
         <v>53</v>
-      </c>
-      <c t="s" s="1" r="E20">
-        <v>54</v>
       </c>
     </row>
     <row r="21">
       <c t="s" s="1" r="A21">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c t="s" s="1" r="C21">
         <v>55</v>
@@ -695,100 +746,168 @@
     </row>
     <row r="22">
       <c t="s" s="1" r="A22">
-        <v>47</v>
+        <v>57</v>
+      </c>
+      <c t="s" s="1" r="B22">
+        <v>58</v>
+      </c>
+      <c t="s" s="1" r="C22">
+        <v>59</v>
+      </c>
+      <c t="s" s="1" r="E22">
+        <v>60</v>
       </c>
     </row>
     <row r="23">
       <c t="s" s="1" r="A23">
-        <v>21</v>
-      </c>
-      <c t="s" s="1" r="E23">
-        <v>57</v>
-      </c>
-      <c t="s" s="1" r="G23">
-        <v>58</v>
-      </c>
-      <c t="s" s="1" r="H23">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24">
-      <c t="s" s="3" r="A24">
-        <v>60</v>
-      </c>
-      <c s="1" r="E24"/>
+      <c t="s" s="4" r="A24">
+        <v>62</v>
+      </c>
+      <c t="s" r="B24">
+        <v>63</v>
+      </c>
     </row>
     <row r="25">
       <c t="s" s="1" r="A25">
-        <v>61</v>
-      </c>
-      <c t="s" r="C25">
-        <v>62</v>
-      </c>
-      <c r="D25">
-        <v>10</v>
-      </c>
-      <c s="1" r="E25"/>
+        <v>52</v>
+      </c>
     </row>
     <row r="26">
       <c t="s" s="1" r="A26">
-        <v>21</v>
-      </c>
-      <c t="s" r="B26">
-        <v>63</v>
+        <v>7</v>
+      </c>
+      <c t="s" s="1" r="C26">
+        <v>64</v>
       </c>
       <c t="s" s="1" r="E26">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27">
       <c t="s" s="1" r="A27">
-        <v>21</v>
-      </c>
-      <c t="s" r="B27">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c t="s" s="1" r="C27">
+        <v>67</v>
       </c>
       <c t="s" s="1" r="E27">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
-        <v>18</v>
-      </c>
-      <c t="s" r="B28">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c t="s" s="1" r="C28">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c t="s" s="1" r="E28">
-        <v>69</v>
-      </c>
-      <c t="s" s="1" r="I28">
         <v>70</v>
       </c>
     </row>
     <row r="29">
       <c t="s" s="1" r="A29">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30">
+      <c t="s" s="1" r="A30">
+        <v>33</v>
+      </c>
+      <c t="s" s="1" r="E30">
         <v>71</v>
       </c>
-      <c t="s" s="1" r="C29">
+      <c t="s" s="1" r="H30">
         <v>72</v>
       </c>
-      <c t="s" s="1" r="E29">
+      <c t="s" s="1" r="I30">
         <v>73</v>
       </c>
-      <c t="s" r="F29">
+    </row>
+    <row r="31">
+      <c t="s" s="3" r="A31">
         <v>74</v>
       </c>
-      <c t="s" s="1" r="J29">
+      <c s="1" r="E31"/>
+    </row>
+    <row r="32">
+      <c t="s" s="1" r="A32">
         <v>75</v>
       </c>
-      <c s="1" r="K29">
+      <c t="s" r="C32">
+        <v>76</v>
+      </c>
+      <c r="D32">
+        <v>10</v>
+      </c>
+      <c s="1" r="E32"/>
+    </row>
+    <row r="33">
+      <c t="s" s="1" r="A33">
+        <v>33</v>
+      </c>
+      <c t="s" r="B33">
+        <v>77</v>
+      </c>
+      <c t="s" s="1" r="E33">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34">
+      <c t="s" s="1" r="A34">
+        <v>33</v>
+      </c>
+      <c t="s" r="B34">
+        <v>79</v>
+      </c>
+      <c t="s" s="1" r="E34">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35">
+      <c t="s" s="1" r="A35">
+        <v>30</v>
+      </c>
+      <c t="s" r="B35">
+        <v>81</v>
+      </c>
+      <c t="s" s="1" r="C35">
+        <v>82</v>
+      </c>
+      <c t="s" s="1" r="E35">
+        <v>83</v>
+      </c>
+      <c t="s" s="1" r="J35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36">
+      <c t="s" s="1" r="A36">
+        <v>85</v>
+      </c>
+      <c t="s" s="1" r="C36">
+        <v>86</v>
+      </c>
+      <c t="s" s="1" r="E36">
+        <v>87</v>
+      </c>
+      <c t="s" r="F36">
+        <v>88</v>
+      </c>
+      <c r="G36">
+        <v>5</v>
+      </c>
+      <c t="s" s="1" r="K36">
+        <v>89</v>
+      </c>
+      <c s="1" r="L36">
         <v>1</v>
       </c>
-      <c s="1" r="L29">
+      <c s="1" r="M36">
         <v>10</v>
       </c>
     </row>
@@ -812,15 +931,15 @@
         <v>2</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +959,7 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c t="s" s="1" r="B1">
         <v>2</v>
@@ -851,178 +970,189 @@
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>81</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>82</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>85</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c t="s" s="1" r="B6">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>88</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>89</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>90</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c t="s" s="1" r="B9">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>91</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>92</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11">
       <c t="s" r="A11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c t="s" r="B11">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c t="s" r="C11">
-        <v>94</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12">
       <c t="s" r="A12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c t="s" r="B12">
-        <v>31</v>
+        <v>108</v>
       </c>
       <c t="s" r="C12">
-        <v>31</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13">
       <c t="s" r="A13">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c t="s" r="B13">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c t="s" r="C13">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14">
       <c t="s" r="A14">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c t="s" r="B14">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c t="s" r="C14">
-        <v>95</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15">
       <c t="s" r="A15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c t="s" r="B15">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c t="s" r="C15">
-        <v>97</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16">
       <c t="s" r="A16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c t="s" r="B16">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c t="s" r="C16">
-        <v>99</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17">
       <c t="s" r="A17">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c t="s" r="B17">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c t="s" r="C17">
-        <v>100</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18">
+      <c t="s" r="A18">
+        <v>15</v>
+      </c>
+      <c t="s" r="B18">
+        <v>115</v>
+      </c>
+      <c t="s" r="C18">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1041,23 +1171,23 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>102</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c s="1" r="B3">
         <v>1</v>
@@ -1065,10 +1195,10 @@
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>107</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update example form with ODK1 legacy submission keys. Add script to generate simple XForms xml file from formDef.json
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="516" yWindow="504" windowWidth="18876" windowHeight="9204" activeTab="3"/>
+  </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="calculates" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="choices" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="settings" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="calculates" sheetId="2" r:id="rId2"/>
+    <sheet name="choices" sheetId="3" r:id="rId3"/>
+    <sheet name="settings" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="123" count="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="129">
   <si>
     <t>type</t>
   </si>
@@ -383,47 +386,55 @@
   </si>
   <si>
     <t>Example Form</t>
+  </si>
+  <si>
+    <t>xmlRootElementName</t>
+  </si>
+  <si>
+    <t>yourRoot</t>
+  </si>
+  <si>
+    <t>xmlSubmissionUrl</t>
+  </si>
+  <si>
+    <t>https://opendatakit-2.appspot.com/submission</t>
+  </si>
+  <si>
+    <t>MIIBIjANBgkqhkiG8w0BAQEFAAOCAQ8AMIIBCgKCAQEAo93+Dgn3iDleC9XMTDH7ez1MOm/BOt287DgkldNkdvrtdC4oUegx3N8Say9tq47k2EOzeLYkezVnKdtserx+g/+R6pDIOS66bwbH+HoslDEUaZRZ47EipSGC1JhtOp/nQGQCsdVc5q/fPvw8d2rLLi+PQUZPBOiBxUo9h/CFc41hl/quUELmylSdL4O06OAP8OCEDA+tl0C2Ik+uCYMDJLD4m7YVbkV7jJXjtILj+GW+noLriFMRsgg7WKQe2j9fw5+v46nzhokOnDnHh+yGwQMfs/B0jfFAgXllLNjIPlXQf2UVzuxEax6wLCyqUXMIjCPSNfnzDRgFB4Qw3QbJCwIDAQAB</t>
+  </si>
+  <si>
+    <t>xmlBase64RsaPublicKey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -432,9 +443,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -464,743 +473,1081 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="2" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="2" fillId="3" borderId="0" applyFill="1"/>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="3" fillId="4" borderId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="11.57" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col max="1" min="1" customWidth="1" width="27.14"/>
-    <col max="2" min="2" customWidth="1" width="45.86"/>
-    <col max="3" min="3" customWidth="1" width="24.86"/>
-    <col max="4" min="4" customWidth="1" width="19.14"/>
-    <col max="5" min="5" customWidth="1" width="41.86"/>
-    <col max="6" min="6" customWidth="1" width="40.0"/>
-    <col max="8" min="8" customWidth="1" width="20.57"/>
-    <col max="9" min="9" customWidth="1" width="13.0"/>
-    <col max="10" min="10" customWidth="1" width="15.86"/>
-    <col max="11" min="11" customWidth="1" width="18.29"/>
-    <col max="12" min="12" customWidth="1" width="18.43"/>
-    <col max="13" min="13" customWidth="1" width="19.0"/>
-    <col max="14" min="14" customWidth="1" width="27.0"/>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="45.88671875" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="41.88671875" customWidth="1"/>
+    <col min="6" max="6" width="40" customWidth="1"/>
+    <col min="8" max="8" width="20.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="1" r="E1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="1" r="F1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="G1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="1" r="H1">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="1" r="I1">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="1" r="J1">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="1" r="K1">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="1" r="L1">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="1" r="M1">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="1" r="N1">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row ht="18.0" r="2" customHeight="1">
-      <c t="s" s="1" r="A2">
+    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="E2">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3">
-      <c t="s" s="2" r="A3">
+    <row r="3" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="1" r="B3">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4">
-      <c t="s" r="A4">
+    <row r="4" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c t="s" r="C4">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c t="s" r="E4">
+      <c r="E4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5">
-      <c t="s" r="A5">
+    <row r="5" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c t="s" r="C5">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c t="s" r="E5">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6">
-      <c t="s" r="A6">
+    <row r="6" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="C6">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c t="s" r="E6">
+      <c r="E6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7">
-      <c t="s" r="A7">
+    <row r="7" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c t="s" r="C7">
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c t="s" r="E7">
+      <c r="E7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8">
-      <c t="s" s="3" r="A8">
+    <row r="8" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9">
-      <c t="s" s="2" r="A9">
+    <row r="9" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
-      <c t="s" s="1" r="B9">
+      <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10">
-      <c t="s" s="1" r="A10">
+    <row r="10" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
-      <c t="s" s="1" r="C10">
+      <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="E10">
+      <c r="E10" s="1" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="1" r="F10">
+      <c r="F10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11">
-      <c t="s" s="1" r="A11">
+    <row r="11" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
-      <c t="s" s="1" r="E11">
+      <c r="E11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row ht="18.0" r="12" customHeight="1">
-      <c t="s" s="3" r="A12">
+    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row ht="18.0" r="13" customHeight="1">
-      <c t="s" s="2" r="A13">
+    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="1" r="B13">
+      <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row ht="18.0" r="14" customHeight="1">
-      <c t="s" s="1" r="A14">
+    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
-      <c t="s" r="C14">
+      <c r="C14" t="s">
         <v>39</v>
       </c>
-      <c t="s" s="1" r="E14">
+      <c r="E14" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row ht="18.0" r="15" customHeight="1">
-      <c t="s" s="1" r="A15">
+    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c t="s" r="C15">
+      <c r="C15" t="s">
         <v>41</v>
       </c>
-      <c t="s" s="1" r="E15">
+      <c r="E15" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row ht="18.0" r="16" customHeight="1">
-      <c t="s" s="1" r="A16">
+    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
-      <c t="s" r="C16">
+      <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="1" r="E16">
+      <c r="E16" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17">
-      <c t="s" s="1" r="A17">
+    <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="1" r="C17">
+      <c r="C17" s="1" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="1" r="E17">
+      <c r="E17" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row ht="18.0" r="18" customHeight="1">
-      <c t="s" s="3" r="A18">
+    <row r="18" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>47</v>
       </c>
-      <c s="1" r="C18"/>
-    </row>
-    <row ht="18.0" r="19" customHeight="1">
-      <c t="s" s="1" r="A19">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
-      <c t="s" r="B19">
+      <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="1" r="C19">
+      <c r="C19" s="1" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="1" r="E19">
+      <c r="E19" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
+    <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
-      <c t="s" r="B20">
+      <c r="B20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21">
-      <c t="s" s="1" r="A21">
+    <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
-      <c t="s" s="1" r="C21">
+      <c r="C21" s="1" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="1" r="E21">
+      <c r="E21" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22">
-      <c t="s" s="1" r="A22">
+    <row r="22" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
-      <c t="s" s="1" r="B22">
+      <c r="B22" s="1" t="s">
         <v>58</v>
       </c>
-      <c t="s" s="1" r="C22">
+      <c r="C22" s="1" t="s">
         <v>59</v>
       </c>
-      <c t="s" s="1" r="E22">
+      <c r="E22" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23">
-      <c t="s" s="1" r="A23">
+    <row r="23" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24">
-      <c t="s" s="4" r="A24">
+    <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>62</v>
       </c>
-      <c t="s" r="B24">
+      <c r="B24" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25">
-      <c t="s" s="1" r="A25">
+    <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26">
-      <c t="s" s="1" r="A26">
+    <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="1" r="C26">
+      <c r="C26" s="1" t="s">
         <v>64</v>
       </c>
-      <c t="s" s="1" r="E26">
+      <c r="E26" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27">
-      <c t="s" s="1" r="A27">
+    <row r="27" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>66</v>
       </c>
-      <c t="s" s="1" r="C27">
+      <c r="C27" s="1" t="s">
         <v>67</v>
       </c>
-      <c t="s" s="1" r="E27">
+      <c r="E27" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="28">
-      <c t="s" s="1" r="A28">
+    <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="1" r="C28">
+      <c r="C28" s="1" t="s">
         <v>69</v>
       </c>
-      <c t="s" s="1" r="E28">
+      <c r="E28" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="29">
-      <c t="s" s="1" r="A29">
+    <row r="29" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30">
-      <c t="s" s="1" r="A30">
+    <row r="30" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
-      <c t="s" s="1" r="E30">
+      <c r="E30" s="1" t="s">
         <v>71</v>
       </c>
-      <c t="s" s="1" r="H30">
+      <c r="H30" s="1" t="s">
         <v>72</v>
       </c>
-      <c t="s" s="1" r="I30">
+      <c r="I30" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31">
-      <c t="s" s="3" r="A31">
+    <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>74</v>
       </c>
-      <c s="1" r="E31"/>
-    </row>
-    <row r="32">
-      <c t="s" s="1" r="A32">
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>75</v>
       </c>
-      <c t="s" r="C32">
+      <c r="C32" t="s">
         <v>76</v>
       </c>
       <c r="D32">
         <v>10</v>
       </c>
-      <c s="1" r="E32"/>
-    </row>
-    <row r="33">
-      <c t="s" s="1" r="A33">
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-      <c t="s" r="B33">
+      <c r="B33" t="s">
         <v>77</v>
       </c>
-      <c t="s" s="1" r="E33">
+      <c r="E33" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34">
-      <c t="s" s="1" r="A34">
+    <row r="34" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
-      <c t="s" r="B34">
+      <c r="B34" t="s">
         <v>79</v>
       </c>
-      <c t="s" s="1" r="E34">
+      <c r="E34" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="35">
-      <c t="s" s="1" r="A35">
+    <row r="35" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>30</v>
       </c>
-      <c t="s" r="B35">
+      <c r="B35" t="s">
         <v>81</v>
       </c>
-      <c t="s" s="1" r="C35">
+      <c r="C35" s="1" t="s">
         <v>82</v>
       </c>
-      <c t="s" s="1" r="E35">
+      <c r="E35" s="1" t="s">
         <v>83</v>
       </c>
-      <c t="s" s="1" r="J35">
+      <c r="J35" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36">
-      <c t="s" s="1" r="A36">
+    <row r="36" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>85</v>
       </c>
-      <c t="s" s="1" r="C36">
+      <c r="C36" s="1" t="s">
         <v>86</v>
       </c>
-      <c t="s" s="1" r="E36">
+      <c r="E36" s="1" t="s">
         <v>87</v>
       </c>
-      <c t="s" r="F36">
+      <c r="F36" t="s">
         <v>88</v>
       </c>
       <c r="G36">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="K36">
+      <c r="K36" s="1" t="s">
         <v>89</v>
       </c>
-      <c s="1" r="L36">
+      <c r="L36" s="1">
         <v>1</v>
       </c>
-      <c s="1" r="M36">
+      <c r="M36" s="1">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="9.14" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col max="1" min="1" customWidth="1" width="21.43"/>
-    <col max="2" min="2" customWidth="1" width="49.43"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="49.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" s="1" r="A2">
+    <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
-      <c t="s" s="1" r="B2">
+      <c r="B2" s="1" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="11.57" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col max="2" min="2" customWidth="1" width="18.14"/>
-    <col max="3" min="3" customWidth="1" width="15.86"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>93</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" s="1" r="A2">
+    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>94</v>
       </c>
-      <c t="s" s="1" r="B2">
+      <c r="B2" s="1" t="s">
         <v>95</v>
       </c>
-      <c t="s" s="1" r="C2">
+      <c r="C2" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="3">
-      <c t="s" s="1" r="A3">
+    <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>94</v>
       </c>
-      <c t="s" s="1" r="B3">
+      <c r="B3" s="1" t="s">
         <v>96</v>
       </c>
-      <c t="s" s="1" r="C3">
+      <c r="C3" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="4">
-      <c t="s" s="1" r="A4">
+    <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="1" r="B4">
+      <c r="B4" s="1" t="s">
         <v>98</v>
       </c>
-      <c t="s" s="1" r="C4">
+      <c r="C4" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5">
-      <c t="s" s="1" r="A5">
+    <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="1" r="B5">
+      <c r="B5" s="1" t="s">
         <v>100</v>
       </c>
-      <c t="s" s="1" r="C5">
+      <c r="C5" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
+    <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="1" r="B6">
+      <c r="B6" s="1" t="s">
         <v>102</v>
       </c>
-      <c t="s" s="1" r="C6">
+      <c r="C6" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7">
-      <c t="s" s="1" r="A7">
+    <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="1" r="B7">
+      <c r="B7" s="1" t="s">
         <v>103</v>
       </c>
-      <c t="s" s="1" r="C7">
+      <c r="C7" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8">
-      <c t="s" s="1" r="A8">
+    <row r="8" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="1" r="B8">
+      <c r="B8" s="1" t="s">
         <v>104</v>
       </c>
-      <c t="s" s="1" r="C8">
+      <c r="C8" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9">
-      <c t="s" s="1" r="A9">
+    <row r="9" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="1" r="B9">
+      <c r="B9" s="1" t="s">
         <v>105</v>
       </c>
-      <c t="s" s="1" r="C9">
+      <c r="C9" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="10">
-      <c t="s" s="1" r="A10">
+    <row r="10" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>97</v>
       </c>
-      <c t="s" s="1" r="B10">
+      <c r="B10" s="1" t="s">
         <v>106</v>
       </c>
-      <c t="s" s="1" r="C10">
+      <c r="C10" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11">
-      <c t="s" r="A11">
+    <row r="11" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B11">
+      <c r="B11" t="s">
         <v>107</v>
       </c>
-      <c t="s" r="C11">
+      <c r="C11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12">
-      <c t="s" r="A12">
+    <row r="12" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B12">
+      <c r="B12" t="s">
         <v>108</v>
       </c>
-      <c t="s" r="C12">
+      <c r="C12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13">
-      <c t="s" r="A13">
+    <row r="13" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B13">
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c t="s" r="C13">
+      <c r="C13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14">
-      <c t="s" r="A14">
+    <row r="14" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B14">
+      <c r="B14" t="s">
         <v>48</v>
       </c>
-      <c t="s" r="C14">
+      <c r="C14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15">
-      <c t="s" r="A15">
+    <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B15">
+      <c r="B15" t="s">
         <v>110</v>
       </c>
-      <c t="s" r="C15">
+      <c r="C15" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="16">
-      <c t="s" r="A16">
+    <row r="16" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B16">
+      <c r="B16" t="s">
         <v>111</v>
       </c>
-      <c t="s" r="C16">
+      <c r="C16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17">
-      <c t="s" r="A17">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B17">
+      <c r="B17" t="s">
         <v>113</v>
       </c>
-      <c t="s" r="C17">
+      <c r="C17" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18">
-      <c t="s" r="A18">
+    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B18">
+      <c r="B18" t="s">
         <v>115</v>
       </c>
-      <c t="s" r="C18">
+      <c r="C18" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="11.57" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col max="2" min="2" customWidth="1" width="13.57"/>
+    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>116</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" s="1" r="A2">
+    <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>118</v>
       </c>
-      <c t="s" s="1" r="B2">
+      <c r="B2" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3">
-      <c t="s" s="1" r="A3">
+    <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>120</v>
       </c>
-      <c s="1" r="B3">
+      <c r="B3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
-      <c t="s" s="1" r="A4">
+    <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>121</v>
       </c>
-      <c t="s" s="1" r="B4">
+      <c r="B4" s="1" t="s">
         <v>122</v>
       </c>
     </row>
+    <row r="5" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding error prompt type + fixing UI issues with button size, datepicker, and intent launching
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125" count="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="135" count="190">
   <si>
     <t>type</t>
   </si>
@@ -68,6 +68,30 @@
     <t>Which examples would you like to see?</t>
   </si>
   <si>
+    <t>goto error_end</t>
+  </si>
+  <si>
+    <t>not(selected(data('examples'), 'error'))</t>
+  </si>
+  <si>
+    <t>select_one yesno</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>Trigger an error on the next screen?</t>
+  </si>
+  <si>
+    <t>Error prompts are useful for finding bugs in forms with lots of branching.</t>
+  </si>
+  <si>
+    <t>selected(data('error'), 'yes')</t>
+  </si>
+  <si>
+    <t>label error_end</t>
+  </si>
+  <si>
     <t>goto intents_end</t>
   </si>
   <si>
@@ -86,6 +110,15 @@
     <t>Record blood oxygen level</t>
   </si>
   <si>
+    <t>breathcounter</t>
+  </si>
+  <si>
+    <t>breathcount</t>
+  </si>
+  <si>
+    <t>Record breath count</t>
+  </si>
+  <si>
     <t>picture</t>
   </si>
   <si>
@@ -186,9 +219,6 @@
   </si>
   <si>
     <t>Which continents have you visited?</t>
-  </si>
-  <si>
-    <t>select_one yesno</t>
   </si>
   <si>
     <t>calculates.ask_about_seattle()</t>
@@ -577,344 +607,390 @@
       </c>
     </row>
     <row r="4">
-      <c t="s" r="A4">
+      <c t="s" s="1" r="A4">
         <v>19</v>
       </c>
       <c t="s" r="C4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c t="s" r="E4">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c t="s" r="F4">
+        <v>22</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>21</v>
-      </c>
-      <c t="s" r="C5">
-        <v>21</v>
-      </c>
-      <c t="s" r="E5">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c t="s" r="B5">
+        <v>23</v>
       </c>
     </row>
     <row r="6">
-      <c t="s" r="A6">
+      <c t="s" s="3" r="A6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c t="s" s="2" r="A7">
+        <v>25</v>
+      </c>
+      <c t="s" s="1" r="B7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8">
+      <c t="s" r="A8">
+        <v>27</v>
+      </c>
+      <c t="s" r="C8">
+        <v>27</v>
+      </c>
+      <c t="s" r="E8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9">
+      <c t="s" r="A9">
+        <v>29</v>
+      </c>
+      <c t="s" r="C9">
+        <v>29</v>
+      </c>
+      <c t="s" r="E9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" r="A10">
+        <v>31</v>
+      </c>
+      <c t="s" r="C10">
+        <v>32</v>
+      </c>
+      <c t="s" r="E10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11">
+      <c t="s" r="A11">
         <v>8</v>
       </c>
-      <c t="s" r="C6">
-        <v>23</v>
-      </c>
-      <c t="s" r="E6">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7">
-      <c t="s" r="A7">
+      <c t="s" r="C11">
+        <v>34</v>
+      </c>
+      <c t="s" r="E11">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" r="A12">
         <v>7</v>
       </c>
-      <c t="s" r="C7">
-        <v>25</v>
-      </c>
-      <c t="s" r="E7">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8">
-      <c t="s" s="3" r="A8">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9">
-      <c t="s" s="2" r="A9">
-        <v>28</v>
-      </c>
-      <c t="s" s="1" r="B9">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10">
-      <c t="s" s="1" r="A10">
-        <v>30</v>
-      </c>
-      <c t="s" s="1" r="C10">
+      <c t="s" r="C12">
+        <v>36</v>
+      </c>
+      <c t="s" r="E12">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" s="3" r="A13">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14">
+      <c t="s" s="2" r="A14">
+        <v>39</v>
+      </c>
+      <c t="s" s="1" r="B14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" s="1" r="A15">
+        <v>41</v>
+      </c>
+      <c t="s" s="1" r="C15">
         <v>2</v>
-      </c>
-      <c t="s" s="1" r="E10">
-        <v>31</v>
-      </c>
-      <c t="s" s="1" r="F10">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11">
-      <c t="s" s="1" r="A11">
-        <v>33</v>
-      </c>
-      <c t="s" s="1" r="E11">
-        <v>34</v>
-      </c>
-    </row>
-    <row ht="18.0" r="12" customHeight="1">
-      <c t="s" s="3" r="A12">
-        <v>35</v>
-      </c>
-    </row>
-    <row ht="18.0" r="13" customHeight="1">
-      <c t="s" s="2" r="A13">
-        <v>36</v>
-      </c>
-      <c t="s" s="1" r="B13">
-        <v>37</v>
-      </c>
-    </row>
-    <row ht="18.0" r="14" customHeight="1">
-      <c t="s" s="1" r="A14">
-        <v>38</v>
-      </c>
-      <c t="s" r="C14">
-        <v>39</v>
-      </c>
-      <c t="s" s="1" r="E14">
-        <v>40</v>
-      </c>
-    </row>
-    <row ht="18.0" r="15" customHeight="1">
-      <c t="s" s="1" r="A15">
-        <v>33</v>
-      </c>
-      <c t="s" r="C15">
-        <v>41</v>
       </c>
       <c t="s" s="1" r="E15">
         <v>42</v>
       </c>
-    </row>
-    <row ht="18.0" r="16" customHeight="1">
+      <c t="s" s="1" r="F15">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16">
       <c t="s" s="1" r="A16">
-        <v>43</v>
-      </c>
-      <c t="s" r="C16">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c t="s" s="1" r="E16">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17">
-      <c t="s" s="1" r="A17">
         <v>45</v>
       </c>
-      <c t="s" s="1" r="C17">
-        <v>45</v>
-      </c>
-      <c t="s" s="1" r="E17">
+    </row>
+    <row ht="18.0" r="17" customHeight="1">
+      <c t="s" s="3" r="A17">
         <v>46</v>
       </c>
     </row>
     <row ht="18.0" r="18" customHeight="1">
-      <c t="s" s="3" r="A18">
+      <c t="s" s="2" r="A18">
         <v>47</v>
       </c>
-      <c s="1" r="C18"/>
+      <c t="s" s="1" r="B18">
+        <v>48</v>
+      </c>
     </row>
     <row ht="18.0" r="19" customHeight="1">
       <c t="s" s="1" r="A19">
-        <v>48</v>
-      </c>
-      <c t="s" r="B19">
         <v>49</v>
       </c>
-      <c t="s" s="1" r="C19">
+      <c t="s" r="C19">
         <v>50</v>
       </c>
       <c t="s" s="1" r="E19">
         <v>51</v>
       </c>
     </row>
-    <row r="20">
+    <row ht="18.0" r="20" customHeight="1">
       <c t="s" s="1" r="A20">
+        <v>44</v>
+      </c>
+      <c t="s" r="C20">
         <v>52</v>
       </c>
-      <c t="s" r="B20">
+      <c t="s" s="1" r="E20">
         <v>53</v>
       </c>
     </row>
-    <row r="21">
+    <row ht="18.0" r="21" customHeight="1">
       <c t="s" s="1" r="A21">
         <v>54</v>
       </c>
-      <c t="s" s="1" r="C21">
+      <c t="s" r="C21">
+        <v>54</v>
+      </c>
+      <c t="s" s="1" r="E21">
         <v>55</v>
-      </c>
-      <c t="s" s="1" r="E21">
-        <v>56</v>
       </c>
     </row>
     <row r="22">
       <c t="s" s="1" r="A22">
+        <v>56</v>
+      </c>
+      <c t="s" s="1" r="C22">
+        <v>56</v>
+      </c>
+      <c t="s" s="1" r="E22">
         <v>57</v>
       </c>
-      <c t="s" s="1" r="B22">
+    </row>
+    <row ht="18.0" r="23" customHeight="1">
+      <c t="s" s="3" r="A23">
         <v>58</v>
       </c>
-      <c t="s" s="1" r="C22">
+      <c s="1" r="C23"/>
+    </row>
+    <row ht="18.0" r="24" customHeight="1">
+      <c t="s" s="1" r="A24">
         <v>59</v>
       </c>
-      <c t="s" s="1" r="E22">
+      <c t="s" r="B24">
         <v>60</v>
       </c>
-    </row>
-    <row r="23">
-      <c t="s" s="1" r="A23">
+      <c t="s" s="1" r="C24">
         <v>61</v>
       </c>
-    </row>
-    <row r="24">
-      <c t="s" s="4" r="A24">
+      <c t="s" s="1" r="E24">
         <v>62</v>
-      </c>
-      <c t="s" r="B24">
-        <v>63</v>
       </c>
     </row>
     <row r="25">
       <c t="s" s="1" r="A25">
-        <v>52</v>
+        <v>63</v>
+      </c>
+      <c t="s" r="B25">
+        <v>64</v>
       </c>
     </row>
     <row r="26">
       <c t="s" s="1" r="A26">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c t="s" s="1" r="C26">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c t="s" s="1" r="E26">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27">
       <c t="s" s="1" r="A27">
-        <v>66</v>
+        <v>19</v>
+      </c>
+      <c t="s" s="1" r="B27">
+        <v>68</v>
       </c>
       <c t="s" s="1" r="C27">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c t="s" s="1" r="E27">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
-        <v>8</v>
-      </c>
-      <c t="s" s="1" r="C28">
-        <v>69</v>
-      </c>
-      <c t="s" s="1" r="E28">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29">
-      <c t="s" s="1" r="A29">
-        <v>61</v>
+      <c t="s" s="4" r="A29">
+        <v>72</v>
+      </c>
+      <c t="s" r="B29">
+        <v>73</v>
       </c>
     </row>
     <row r="30">
       <c t="s" s="1" r="A30">
-        <v>33</v>
-      </c>
-      <c t="s" s="1" r="E30">
-        <v>71</v>
-      </c>
-      <c t="s" s="1" r="H30">
-        <v>72</v>
-      </c>
-      <c t="s" s="1" r="I30">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31">
-      <c t="s" s="3" r="A31">
+      <c t="s" s="1" r="A31">
+        <v>7</v>
+      </c>
+      <c t="s" s="1" r="C31">
         <v>74</v>
       </c>
-      <c s="1" r="E31"/>
+      <c t="s" s="1" r="E31">
+        <v>75</v>
+      </c>
     </row>
     <row r="32">
       <c t="s" s="1" r="A32">
-        <v>75</v>
-      </c>
-      <c t="s" r="C32">
         <v>76</v>
       </c>
-      <c r="D32">
-        <v>10</v>
-      </c>
-      <c s="1" r="E32"/>
+      <c t="s" s="1" r="C32">
+        <v>77</v>
+      </c>
+      <c t="s" s="1" r="E32">
+        <v>78</v>
+      </c>
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>33</v>
-      </c>
-      <c t="s" r="B33">
-        <v>77</v>
+        <v>8</v>
+      </c>
+      <c t="s" s="1" r="C33">
+        <v>79</v>
       </c>
       <c t="s" s="1" r="E33">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34">
       <c t="s" s="1" r="A34">
-        <v>33</v>
-      </c>
-      <c t="s" r="B34">
-        <v>79</v>
-      </c>
-      <c t="s" s="1" r="E34">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35">
       <c t="s" s="1" r="A35">
-        <v>30</v>
-      </c>
-      <c t="s" r="B35">
+        <v>44</v>
+      </c>
+      <c t="s" s="1" r="E35">
         <v>81</v>
       </c>
-      <c t="s" s="1" r="C35">
+      <c t="s" s="1" r="H35">
         <v>82</v>
       </c>
-      <c t="s" s="1" r="E35">
+      <c t="s" s="1" r="I35">
         <v>83</v>
       </c>
-      <c t="s" s="1" r="J35">
+    </row>
+    <row r="36">
+      <c t="s" s="3" r="A36">
         <v>84</v>
       </c>
-    </row>
-    <row r="36">
-      <c t="s" s="1" r="A36">
+      <c s="1" r="E36"/>
+    </row>
+    <row r="37">
+      <c t="s" s="1" r="A37">
         <v>85</v>
       </c>
-      <c t="s" s="1" r="C36">
+      <c t="s" r="C37">
         <v>86</v>
       </c>
-      <c t="s" s="1" r="E36">
+      <c r="D37">
+        <v>10</v>
+      </c>
+      <c s="1" r="E37"/>
+    </row>
+    <row r="38">
+      <c t="s" s="1" r="A38">
+        <v>44</v>
+      </c>
+      <c t="s" r="B38">
         <v>87</v>
       </c>
-      <c t="s" r="F36">
+      <c t="s" s="1" r="E38">
         <v>88</v>
       </c>
-      <c r="G36">
+    </row>
+    <row r="39">
+      <c t="s" s="1" r="A39">
+        <v>44</v>
+      </c>
+      <c t="s" r="B39">
+        <v>89</v>
+      </c>
+      <c t="s" s="1" r="E39">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40">
+      <c t="s" s="1" r="A40">
+        <v>41</v>
+      </c>
+      <c t="s" r="B40">
+        <v>91</v>
+      </c>
+      <c t="s" s="1" r="C40">
+        <v>92</v>
+      </c>
+      <c t="s" s="1" r="E40">
+        <v>93</v>
+      </c>
+      <c t="s" s="1" r="J40">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41">
+      <c t="s" s="1" r="A41">
+        <v>95</v>
+      </c>
+      <c t="s" s="1" r="C41">
+        <v>96</v>
+      </c>
+      <c t="s" s="1" r="E41">
+        <v>97</v>
+      </c>
+      <c t="s" r="F41">
+        <v>98</v>
+      </c>
+      <c r="G41">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="K36">
-        <v>89</v>
-      </c>
-      <c s="1" r="L36">
+      <c t="s" s="1" r="K41">
+        <v>99</v>
+      </c>
+      <c s="1" r="L41">
         <v>1</v>
       </c>
-      <c s="1" r="M36">
+      <c s="1" r="M41">
         <v>10</v>
       </c>
     </row>
@@ -938,15 +1014,15 @@
         <v>2</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -965,15 +1041,15 @@
         <v>2</v>
       </c>
       <c t="s" r="B1">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c t="s" r="B2">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -993,7 +1069,7 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c t="s" s="1" r="B1">
         <v>2</v>
@@ -1004,101 +1080,101 @@
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>97</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>101</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="B6">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>104</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="B9">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>107</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>108</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11">
@@ -1106,10 +1182,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B11">
-        <v>109</v>
+        <v>20</v>
       </c>
       <c t="s" r="C11">
-        <v>109</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
@@ -1117,10 +1193,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B12">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c t="s" r="C12">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13">
@@ -1128,10 +1204,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B13">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c t="s" r="C13">
-        <v>45</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14">
@@ -1139,10 +1215,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B14">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c t="s" r="C14">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15">
@@ -1150,10 +1226,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B15">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c t="s" r="C15">
-        <v>112</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16">
@@ -1161,10 +1237,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B16">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c t="s" r="C16">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17">
@@ -1172,10 +1248,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B17">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c t="s" r="C17">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18">
@@ -1183,10 +1259,21 @@
         <v>15</v>
       </c>
       <c t="s" r="B18">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c t="s" r="C18">
-        <v>117</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19">
+      <c t="s" r="A19">
+        <v>15</v>
+      </c>
+      <c t="s" r="B19">
+        <v>127</v>
+      </c>
+      <c t="s" r="C19">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1205,23 +1292,23 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c s="1" r="B3">
         <v>1</v>
@@ -1229,10 +1316,10 @@
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaning up builder and making it possible to package custom prompt types with forms.
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="135" count="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="135" count="192">
   <si>
     <t>type</t>
   </si>
@@ -1052,6 +1052,14 @@
         <v>104</v>
       </c>
     </row>
+    <row r="3">
+      <c t="s" r="A3">
+        <v>32</v>
+      </c>
+      <c t="s" r="B3">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
removing custom prompt types from example form and adding error to promptTypes
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="135" count="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="132" count="186">
   <si>
     <t>type</t>
   </si>
@@ -104,232 +104,223 @@
     <t>Scan a barcode</t>
   </si>
   <si>
+    <t>picture</t>
+  </si>
+  <si>
+    <t>Take a picture</t>
+  </si>
+  <si>
+    <t>recording</t>
+  </si>
+  <si>
+    <t>Make a recording</t>
+  </si>
+  <si>
+    <t>label intents_end</t>
+  </si>
+  <si>
+    <t>goto dynamic_label_end</t>
+  </si>
+  <si>
+    <t>not(selected(data('examples'), 'dynamic_label'))</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Enter your name</t>
+  </si>
+  <si>
+    <t>Please use your full name</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Hello {{name.value}}</t>
+  </si>
+  <si>
+    <t>label dynamic_label_end</t>
+  </si>
+  <si>
+    <t>goto datetime_end</t>
+  </si>
+  <si>
+    <t>not(selected(data('examples'), 'datetime'))</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>born</t>
+  </si>
+  <si>
+    <t>When were you born?</t>
+  </si>
+  <si>
+    <t>data('born').getDay() === now().getDay() &amp;&amp; data('born').getMonth() === now().getMonth()</t>
+  </si>
+  <si>
+    <t>Happy Birthday!</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>What time is it?</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>When will you be available for a follow up survey?</t>
+  </si>
+  <si>
+    <t>label datetime_end</t>
+  </si>
+  <si>
+    <t>geopoint</t>
+  </si>
+  <si>
+    <t>selected(data('examples'), 'geopoint')</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Record your location:</t>
+  </si>
+  <si>
+    <t>begin screen</t>
+  </si>
+  <si>
+    <t>selected(data('examples'), 'screen_group')</t>
+  </si>
+  <si>
+    <t>select continents</t>
+  </si>
+  <si>
+    <t>visited_continents</t>
+  </si>
+  <si>
+    <t>Which continents have you visited?</t>
+  </si>
+  <si>
+    <t>calculates.ask_about_seattle()</t>
+  </si>
+  <si>
+    <t>visited_seattle</t>
+  </si>
+  <si>
+    <t>Have you visited Seattle?</t>
+  </si>
+  <si>
+    <t>end screen</t>
+  </si>
+  <si>
+    <t>goto media_end</t>
+  </si>
+  <si>
+    <t>not(selected(data('examples'), 'media'))</t>
+  </si>
+  <si>
+    <t>audio_test</t>
+  </si>
+  <si>
+    <t>Make a recording:</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>video_test</t>
+  </si>
+  <si>
+    <t>Take a video:</t>
+  </si>
+  <si>
+    <t>image_test</t>
+  </si>
+  <si>
+    <t>Take a picture:</t>
+  </si>
+  <si>
+    <t>This prompt shows how to embed media in labels.</t>
+  </si>
+  <si>
+    <t>audio/carrioncrow.mp3</t>
+  </si>
+  <si>
+    <t>img/dolphin.png</t>
+  </si>
+  <si>
+    <t>label media_end</t>
+  </si>
+  <si>
+    <t>with_next</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>selected(data('examples'), 'assignment')</t>
+  </si>
+  <si>
+    <t>Assigning a value of 10 to x.</t>
+  </si>
+  <si>
+    <t>data('x') === 10</t>
+  </si>
+  <si>
+    <t>x = {{x.value}}</t>
+  </si>
+  <si>
+    <t>selected(data('examples'), 'custom_template')</t>
+  </si>
+  <si>
+    <t>specialTemplateTest</t>
+  </si>
+  <si>
+    <t>This is a custom template that uses D3.js:</t>
+  </si>
+  <si>
+    <t>test.handlebars</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>How would you rate this survey?</t>
+  </si>
+  <si>
+    <t>1 is very bad. 10 is very good.</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>ask_about_seattle</t>
+  </si>
+  <si>
+    <t>selected(data('visited_continents'), 'NorthAmerica')</t>
+  </si>
+  <si>
+    <t>schema.type</t>
+  </si>
+  <si>
     <t>pulseox</t>
   </si>
   <si>
-    <t>Record blood oxygen level</t>
-  </si>
-  <si>
-    <t>breathcounter</t>
+    <t>string</t>
   </si>
   <si>
     <t>breathcount</t>
-  </si>
-  <si>
-    <t>Record breath count</t>
-  </si>
-  <si>
-    <t>picture</t>
-  </si>
-  <si>
-    <t>Take a picture</t>
-  </si>
-  <si>
-    <t>recording</t>
-  </si>
-  <si>
-    <t>Make a recording</t>
-  </si>
-  <si>
-    <t>label intents_end</t>
-  </si>
-  <si>
-    <t>goto dynamic_label_end</t>
-  </si>
-  <si>
-    <t>not(selected(data('examples'), 'dynamic_label'))</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>Enter your name</t>
-  </si>
-  <si>
-    <t>Please use your full name</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>Hello {{name.value}}</t>
-  </si>
-  <si>
-    <t>label dynamic_label_end</t>
-  </si>
-  <si>
-    <t>goto datetime_end</t>
-  </si>
-  <si>
-    <t>not(selected(data('examples'), 'datetime'))</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>born</t>
-  </si>
-  <si>
-    <t>When were you born?</t>
-  </si>
-  <si>
-    <t>data('born').getDay() === now().getDay() &amp;&amp; data('born').getMonth() === now().getMonth()</t>
-  </si>
-  <si>
-    <t>Happy Birthday!</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>What time is it?</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>When will you be available for a follow up survey?</t>
-  </si>
-  <si>
-    <t>label datetime_end</t>
-  </si>
-  <si>
-    <t>geopoint</t>
-  </si>
-  <si>
-    <t>selected(data('examples'), 'geopoint')</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>Record your location:</t>
-  </si>
-  <si>
-    <t>begin screen</t>
-  </si>
-  <si>
-    <t>selected(data('examples'), 'screen_group')</t>
-  </si>
-  <si>
-    <t>select continents</t>
-  </si>
-  <si>
-    <t>visited_continents</t>
-  </si>
-  <si>
-    <t>Which continents have you visited?</t>
-  </si>
-  <si>
-    <t>calculates.ask_about_seattle()</t>
-  </si>
-  <si>
-    <t>visited_seattle</t>
-  </si>
-  <si>
-    <t>Have you visited Seattle?</t>
-  </si>
-  <si>
-    <t>end screen</t>
-  </si>
-  <si>
-    <t>goto media_end</t>
-  </si>
-  <si>
-    <t>not(selected(data('examples'), 'media'))</t>
-  </si>
-  <si>
-    <t>audio_test</t>
-  </si>
-  <si>
-    <t>Make a recording:</t>
-  </si>
-  <si>
-    <t>video</t>
-  </si>
-  <si>
-    <t>video_test</t>
-  </si>
-  <si>
-    <t>Take a video:</t>
-  </si>
-  <si>
-    <t>image_test</t>
-  </si>
-  <si>
-    <t>Take a picture:</t>
-  </si>
-  <si>
-    <t>This prompt shows how to embed media in labels.</t>
-  </si>
-  <si>
-    <t>audio/carrioncrow.mp3</t>
-  </si>
-  <si>
-    <t>img/dolphin.png</t>
-  </si>
-  <si>
-    <t>label media_end</t>
-  </si>
-  <si>
-    <t>with_next</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>selected(data('examples'), 'assignment')</t>
-  </si>
-  <si>
-    <t>Assigning a value of 10 to x.</t>
-  </si>
-  <si>
-    <t>data('x') === 10</t>
-  </si>
-  <si>
-    <t>x = {{x.value}}</t>
-  </si>
-  <si>
-    <t>selected(data('examples'), 'custom_template')</t>
-  </si>
-  <si>
-    <t>specialTemplateTest</t>
-  </si>
-  <si>
-    <t>This is a custom template that uses D3.js:</t>
-  </si>
-  <si>
-    <t>test.handlebars</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>rating</t>
-  </si>
-  <si>
-    <t>How would you rate this survey?</t>
-  </si>
-  <si>
-    <t>1 is very bad. 10 is very good.</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
-    <t>calculation</t>
-  </si>
-  <si>
-    <t>ask_about_seattle</t>
-  </si>
-  <si>
-    <t>selected(data('visited_continents'), 'NorthAmerica')</t>
-  </si>
-  <si>
-    <t>schema.type</t>
-  </si>
-  <si>
-    <t>string</t>
   </si>
   <si>
     <t>list_name</t>
@@ -654,7 +645,7 @@
     </row>
     <row r="9">
       <c t="s" r="A9">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c t="s" r="C9">
         <v>29</v>
@@ -665,82 +656,82 @@
     </row>
     <row r="10">
       <c t="s" r="A10">
+        <v>7</v>
+      </c>
+      <c t="s" r="C10">
         <v>31</v>
       </c>
-      <c t="s" r="C10">
+      <c t="s" r="E10">
         <v>32</v>
       </c>
-      <c t="s" r="E10">
+    </row>
+    <row r="11">
+      <c t="s" s="3" r="A11">
         <v>33</v>
       </c>
     </row>
-    <row r="11">
-      <c t="s" r="A11">
-        <v>8</v>
-      </c>
-      <c t="s" r="C11">
+    <row r="12">
+      <c t="s" s="2" r="A12">
         <v>34</v>
       </c>
-      <c t="s" r="E11">
+      <c t="s" s="1" r="B12">
         <v>35</v>
       </c>
     </row>
-    <row r="12">
-      <c t="s" r="A12">
-        <v>7</v>
-      </c>
-      <c t="s" r="C12">
+    <row r="13">
+      <c t="s" s="1" r="A13">
         <v>36</v>
       </c>
-      <c t="s" r="E12">
+      <c t="s" s="1" r="C13">
+        <v>2</v>
+      </c>
+      <c t="s" s="1" r="E13">
         <v>37</v>
       </c>
-    </row>
-    <row r="13">
-      <c t="s" s="3" r="A13">
+      <c t="s" s="1" r="F13">
         <v>38</v>
       </c>
     </row>
     <row r="14">
-      <c t="s" s="2" r="A14">
+      <c t="s" s="1" r="A14">
         <v>39</v>
       </c>
-      <c t="s" s="1" r="B14">
+      <c t="s" s="1" r="E14">
         <v>40</v>
       </c>
     </row>
-    <row r="15">
-      <c t="s" s="1" r="A15">
+    <row ht="18.0" r="15" customHeight="1">
+      <c t="s" s="3" r="A15">
         <v>41</v>
       </c>
-      <c t="s" s="1" r="C15">
-        <v>2</v>
-      </c>
-      <c t="s" s="1" r="E15">
+    </row>
+    <row ht="18.0" r="16" customHeight="1">
+      <c t="s" s="2" r="A16">
         <v>42</v>
       </c>
-      <c t="s" s="1" r="F15">
+      <c t="s" s="1" r="B16">
         <v>43</v>
       </c>
     </row>
-    <row r="16">
-      <c t="s" s="1" r="A16">
+    <row ht="18.0" r="17" customHeight="1">
+      <c t="s" s="1" r="A17">
         <v>44</v>
       </c>
-      <c t="s" s="1" r="E16">
+      <c t="s" r="C17">
         <v>45</v>
       </c>
-    </row>
-    <row ht="18.0" r="17" customHeight="1">
-      <c t="s" s="3" r="A17">
+      <c t="s" s="1" r="E17">
         <v>46</v>
       </c>
     </row>
     <row ht="18.0" r="18" customHeight="1">
-      <c t="s" s="2" r="A18">
+      <c t="s" s="1" r="A18">
+        <v>39</v>
+      </c>
+      <c t="s" r="B18">
         <v>47</v>
       </c>
-      <c t="s" s="1" r="B18">
+      <c t="s" s="1" r="E18">
         <v>48</v>
       </c>
     </row>
@@ -749,37 +740,35 @@
         <v>49</v>
       </c>
       <c t="s" r="C19">
+        <v>49</v>
+      </c>
+      <c t="s" s="1" r="E19">
         <v>50</v>
       </c>
-      <c t="s" s="1" r="E19">
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
         <v>51</v>
       </c>
-    </row>
-    <row ht="18.0" r="20" customHeight="1">
-      <c t="s" s="1" r="A20">
-        <v>44</v>
-      </c>
-      <c t="s" r="B20">
+      <c t="s" s="1" r="C20">
+        <v>51</v>
+      </c>
+      <c t="s" s="1" r="E20">
         <v>52</v>
       </c>
-      <c t="s" s="1" r="E20">
+    </row>
+    <row ht="18.0" r="21" customHeight="1">
+      <c t="s" s="3" r="A21">
         <v>53</v>
       </c>
-    </row>
-    <row ht="18.0" r="21" customHeight="1">
-      <c t="s" s="1" r="A21">
+      <c s="1" r="C21"/>
+    </row>
+    <row ht="18.0" r="22" customHeight="1">
+      <c t="s" s="1" r="A22">
         <v>54</v>
       </c>
-      <c t="s" r="C21">
-        <v>54</v>
-      </c>
-      <c t="s" s="1" r="E21">
+      <c t="s" r="B22">
         <v>55</v>
-      </c>
-    </row>
-    <row r="22">
-      <c t="s" s="1" r="A22">
-        <v>56</v>
       </c>
       <c t="s" s="1" r="C22">
         <v>56</v>
@@ -788,17 +777,16 @@
         <v>57</v>
       </c>
     </row>
-    <row ht="18.0" r="23" customHeight="1">
-      <c t="s" s="3" r="A23">
+    <row r="23">
+      <c t="s" s="1" r="A23">
         <v>58</v>
       </c>
-      <c s="1" r="C23"/>
-    </row>
-    <row ht="18.0" r="24" customHeight="1">
+      <c t="s" r="B23">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24">
       <c t="s" s="1" r="A24">
-        <v>59</v>
-      </c>
-      <c t="s" r="B24">
         <v>60</v>
       </c>
       <c t="s" s="1" r="C24">
@@ -810,58 +798,61 @@
     </row>
     <row r="25">
       <c t="s" s="1" r="A25">
+        <v>19</v>
+      </c>
+      <c t="s" s="1" r="B25">
         <v>63</v>
       </c>
-      <c t="s" r="B25">
+      <c t="s" s="1" r="C25">
         <v>64</v>
+      </c>
+      <c t="s" s="1" r="E25">
+        <v>65</v>
       </c>
     </row>
     <row r="26">
       <c t="s" s="1" r="A26">
-        <v>65</v>
-      </c>
-      <c t="s" s="1" r="C26">
         <v>66</v>
       </c>
-      <c t="s" s="1" r="E26">
+    </row>
+    <row r="27">
+      <c t="s" s="4" r="A27">
         <v>67</v>
       </c>
-    </row>
-    <row r="27">
-      <c t="s" s="1" r="A27">
-        <v>19</v>
-      </c>
-      <c t="s" s="1" r="B27">
+      <c t="s" r="B27">
         <v>68</v>
-      </c>
-      <c t="s" s="1" r="C27">
-        <v>69</v>
-      </c>
-      <c t="s" s="1" r="E27">
-        <v>70</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29">
-      <c t="s" s="4" r="A29">
-        <v>72</v>
-      </c>
-      <c t="s" r="B29">
-        <v>73</v>
+      <c t="s" s="1" r="A29">
+        <v>7</v>
+      </c>
+      <c t="s" s="1" r="C29">
+        <v>69</v>
+      </c>
+      <c t="s" s="1" r="E29">
+        <v>70</v>
       </c>
     </row>
     <row r="30">
       <c t="s" s="1" r="A30">
-        <v>63</v>
+        <v>71</v>
+      </c>
+      <c t="s" s="1" r="C30">
+        <v>72</v>
+      </c>
+      <c t="s" s="1" r="E30">
+        <v>73</v>
       </c>
     </row>
     <row r="31">
       <c t="s" s="1" r="A31">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c t="s" s="1" r="C31">
         <v>74</v>
@@ -872,125 +863,103 @@
     </row>
     <row r="32">
       <c t="s" s="1" r="A32">
-        <v>76</v>
-      </c>
-      <c t="s" s="1" r="C32">
-        <v>77</v>
-      </c>
-      <c t="s" s="1" r="E32">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>8</v>
-      </c>
-      <c t="s" s="1" r="C33">
+        <v>39</v>
+      </c>
+      <c t="s" s="1" r="E33">
+        <v>76</v>
+      </c>
+      <c t="s" s="1" r="H33">
+        <v>77</v>
+      </c>
+      <c t="s" s="1" r="I33">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34">
+      <c t="s" s="3" r="A34">
         <v>79</v>
       </c>
-      <c t="s" s="1" r="E33">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34">
-      <c t="s" s="1" r="A34">
-        <v>71</v>
-      </c>
+      <c s="1" r="E34"/>
     </row>
     <row r="35">
       <c t="s" s="1" r="A35">
-        <v>44</v>
-      </c>
-      <c t="s" s="1" r="E35">
+        <v>80</v>
+      </c>
+      <c t="s" r="C35">
         <v>81</v>
       </c>
-      <c t="s" s="1" r="H35">
+      <c r="D35">
+        <v>10</v>
+      </c>
+      <c s="1" r="E35"/>
+    </row>
+    <row r="36">
+      <c t="s" s="1" r="A36">
+        <v>39</v>
+      </c>
+      <c t="s" r="B36">
         <v>82</v>
       </c>
-      <c t="s" s="1" r="I35">
+      <c t="s" s="1" r="E36">
         <v>83</v>
       </c>
-    </row>
-    <row r="36">
-      <c t="s" s="3" r="A36">
-        <v>84</v>
-      </c>
-      <c s="1" r="E36"/>
     </row>
     <row r="37">
       <c t="s" s="1" r="A37">
+        <v>39</v>
+      </c>
+      <c t="s" r="B37">
+        <v>84</v>
+      </c>
+      <c t="s" s="1" r="E37">
         <v>85</v>
       </c>
-      <c t="s" r="C37">
-        <v>86</v>
-      </c>
-      <c r="D37">
-        <v>10</v>
-      </c>
-      <c s="1" r="E37"/>
     </row>
     <row r="38">
       <c t="s" s="1" r="A38">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c t="s" r="B38">
+        <v>86</v>
+      </c>
+      <c t="s" s="1" r="C38">
         <v>87</v>
       </c>
       <c t="s" s="1" r="E38">
         <v>88</v>
       </c>
+      <c t="s" s="1" r="J38">
+        <v>89</v>
+      </c>
     </row>
     <row r="39">
       <c t="s" s="1" r="A39">
-        <v>44</v>
-      </c>
-      <c t="s" r="B39">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c t="s" s="1" r="C39">
+        <v>91</v>
       </c>
       <c t="s" s="1" r="E39">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40">
-      <c t="s" s="1" r="A40">
-        <v>41</v>
-      </c>
-      <c t="s" r="B40">
-        <v>91</v>
-      </c>
-      <c t="s" s="1" r="C40">
         <v>92</v>
       </c>
-      <c t="s" s="1" r="E40">
+      <c t="s" r="F39">
         <v>93</v>
       </c>
-      <c t="s" s="1" r="J40">
+      <c r="G39">
+        <v>5</v>
+      </c>
+      <c t="s" s="1" r="K39">
         <v>94</v>
       </c>
-    </row>
-    <row r="41">
-      <c t="s" s="1" r="A41">
-        <v>95</v>
-      </c>
-      <c t="s" s="1" r="C41">
-        <v>96</v>
-      </c>
-      <c t="s" s="1" r="E41">
-        <v>97</v>
-      </c>
-      <c t="s" r="F41">
-        <v>98</v>
-      </c>
-      <c r="G41">
-        <v>5</v>
-      </c>
-      <c t="s" s="1" r="K41">
-        <v>99</v>
-      </c>
-      <c s="1" r="L41">
+      <c s="1" r="L39">
         <v>1</v>
       </c>
-      <c s="1" r="M41">
+      <c s="1" r="M39">
         <v>10</v>
       </c>
     </row>
@@ -1014,15 +983,15 @@
         <v>2</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1041,23 +1010,23 @@
         <v>2</v>
       </c>
       <c t="s" r="B1">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c t="s" r="A2">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c t="s" r="B2">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
       <c t="s" r="A3">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c t="s" r="B3">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1077,7 +1046,7 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c t="s" s="1" r="B1">
         <v>2</v>
@@ -1088,101 +1057,101 @@
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
+        <v>106</v>
+      </c>
+      <c t="s" s="1" r="B5">
         <v>109</v>
       </c>
-      <c t="s" s="1" r="B5">
-        <v>112</v>
-      </c>
       <c t="s" s="1" r="C5">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B6">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B9">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11">
@@ -1201,10 +1170,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B12">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c t="s" r="C12">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13">
@@ -1212,10 +1181,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B13">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c t="s" r="C13">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14">
@@ -1223,10 +1192,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B14">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c t="s" r="C14">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15">
@@ -1234,10 +1203,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B15">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c t="s" r="C15">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16">
@@ -1245,10 +1214,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B16">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c t="s" r="C16">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17">
@@ -1256,10 +1225,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B17">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c t="s" r="C17">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18">
@@ -1267,10 +1236,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B18">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c t="s" r="C18">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19">
@@ -1278,10 +1247,10 @@
         <v>15</v>
       </c>
       <c t="s" r="B19">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c t="s" r="C19">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1300,23 +1269,23 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c s="1" r="B3">
         <v>1</v>
@@ -1324,10 +1293,10 @@
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with select renamed select_multiple
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="516" yWindow="504" windowWidth="18876" windowHeight="8940"/>
+  </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="calculates" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="choices" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="settings" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="calculates" sheetId="2" r:id="rId2"/>
+    <sheet name="choices" sheetId="3" r:id="rId3"/>
+    <sheet name="settings" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="128" count="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="128">
   <si>
     <t>type</t>
   </si>
@@ -196,9 +199,6 @@
     <t>selected(data('examples'), 'screen_group')</t>
   </si>
   <si>
-    <t>select continents</t>
-  </si>
-  <si>
     <t>visited_continents</t>
   </si>
   <si>
@@ -398,46 +398,33 @@
   </si>
   <si>
     <t>Example Form</t>
+  </si>
+  <si>
+    <t>select_multiple continents</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -447,9 +434,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -482,775 +467,1078 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="2" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="2" fillId="3" borderId="0" applyFill="1"/>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="3" fillId="4" borderId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="11.57" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col max="1" min="1" customWidth="1" width="27.14"/>
-    <col max="2" min="2" customWidth="1" width="45.86"/>
-    <col max="3" min="3" customWidth="1" width="24.86"/>
-    <col max="4" min="4" customWidth="1" width="19.14"/>
-    <col max="5" min="5" customWidth="1" width="41.86"/>
-    <col max="6" min="6" customWidth="1" width="40.0"/>
-    <col max="8" min="8" customWidth="1" width="20.57"/>
-    <col max="9" min="9" customWidth="1" width="13.0"/>
-    <col max="10" min="10" customWidth="1" width="15.86"/>
-    <col max="11" min="11" customWidth="1" width="18.29"/>
-    <col max="12" min="12" customWidth="1" width="18.43"/>
-    <col max="13" min="13" customWidth="1" width="19.0"/>
-    <col max="14" min="14" customWidth="1" width="27.0"/>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="45.88671875" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="41.88671875" customWidth="1"/>
+    <col min="6" max="6" width="40" customWidth="1"/>
+    <col min="8" max="8" width="20.5546875" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="1" r="E1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="1" r="F1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="G1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="1" r="H1">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="1" r="I1">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="1" r="J1">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="1" r="K1">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="1" r="L1">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="1" r="M1">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="1" r="N1">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row ht="18.0" r="2" customHeight="1">
-      <c t="s" s="1" r="A2">
+    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c t="s" r="C2">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="E2">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3">
-      <c t="s" s="2" r="A3">
+    <row r="3" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="1" r="B3">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4">
-      <c t="s" s="1" r="A4">
+    <row r="4" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c t="s" r="C4">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c t="s" r="E4">
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c t="s" r="F4">
+      <c r="F4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5">
-      <c t="s" r="A5">
+    <row r="5" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c t="s" r="B5">
+      <c r="B5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6">
-      <c t="s" s="3" r="A6">
+    <row r="6" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7">
-      <c t="s" s="2" r="A7">
+    <row r="7" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="1" r="B7">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8">
-      <c t="s" r="A8">
+    <row r="8" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c t="s" r="C8">
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c t="s" r="E8">
+      <c r="E8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9">
-      <c t="s" r="A9">
+    <row r="9" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c t="s" r="C9">
+      <c r="C9" t="s">
         <v>29</v>
       </c>
-      <c t="s" r="E9">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10">
-      <c t="s" r="A10">
+    <row r="10" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c t="s" r="C10">
+      <c r="C10" t="s">
         <v>31</v>
       </c>
-      <c t="s" r="E10">
+      <c r="E10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11">
-      <c t="s" s="3" r="A11">
+    <row r="11" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12">
-      <c t="s" s="2" r="A12">
+    <row r="12" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
-      <c t="s" s="1" r="B12">
+      <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13">
-      <c t="s" s="1" r="A13">
+    <row r="13" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
-      <c t="s" s="1" r="C13">
+      <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="E13">
+      <c r="E13" s="1" t="s">
         <v>37</v>
       </c>
-      <c t="s" s="1" r="F13">
+      <c r="F13" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14">
-      <c t="s" s="1" r="A14">
+    <row r="14" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
-      <c t="s" s="1" r="E14">
+      <c r="E14" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row ht="18.0" r="15" customHeight="1">
-      <c t="s" s="3" r="A15">
+    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row ht="18.0" r="16" customHeight="1">
-      <c t="s" s="2" r="A16">
+    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
-      <c t="s" s="1" r="B16">
+      <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row ht="18.0" r="17" customHeight="1">
-      <c t="s" s="1" r="A17">
+    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
-      <c t="s" r="C17">
+      <c r="C17" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="1" r="E17">
+      <c r="E17" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row ht="18.0" r="18" customHeight="1">
-      <c t="s" s="1" r="A18">
+    <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
-      <c t="s" r="B18">
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="1" r="E18">
+      <c r="E18" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row ht="18.0" r="19" customHeight="1">
-      <c t="s" s="1" r="A19">
+    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>49</v>
       </c>
-      <c t="s" r="C19">
+      <c r="C19" t="s">
         <v>49</v>
       </c>
-      <c t="s" s="1" r="E19">
+      <c r="E19" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
+    <row r="20" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
-      <c t="s" s="1" r="C20">
+      <c r="C20" s="1" t="s">
         <v>51</v>
       </c>
-      <c t="s" s="1" r="E20">
+      <c r="E20" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row ht="18.0" r="21" customHeight="1">
-      <c t="s" s="3" r="A21">
+    <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>53</v>
       </c>
-      <c s="1" r="C21"/>
-    </row>
-    <row ht="18.0" r="22" customHeight="1">
-      <c t="s" s="1" r="A22">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
-      <c t="s" r="B22">
+      <c r="B22" t="s">
         <v>55</v>
       </c>
-      <c t="s" s="1" r="C22">
+      <c r="C22" s="1" t="s">
         <v>56</v>
       </c>
-      <c t="s" s="1" r="E22">
+      <c r="E22" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23">
-      <c t="s" s="1" r="A23">
+    <row r="23" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
-      <c t="s" r="B23">
+      <c r="B23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24">
-      <c t="s" s="1" r="A24">
+    <row r="24" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>60</v>
       </c>
-      <c t="s" s="1" r="C24">
+      <c r="E24" s="1" t="s">
         <v>61</v>
       </c>
-      <c t="s" s="1" r="E24">
+    </row>
+    <row r="25" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25">
-      <c t="s" s="1" r="A25">
-        <v>19</v>
-      </c>
-      <c t="s" s="1" r="B25">
+      <c r="C25" s="1" t="s">
         <v>63</v>
       </c>
-      <c t="s" s="1" r="C25">
+      <c r="E25" s="1" t="s">
         <v>64</v>
       </c>
-      <c t="s" s="1" r="E25">
+    </row>
+    <row r="26" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26">
-      <c t="s" s="1" r="A26">
+    <row r="27" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="27">
-      <c t="s" s="4" r="A27">
+      <c r="B27" t="s">
         <v>67</v>
       </c>
-      <c t="s" r="B27">
+    </row>
+    <row r="28" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28">
-      <c t="s" s="1" r="A28">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29">
-      <c t="s" s="1" r="A29">
-        <v>7</v>
-      </c>
-      <c t="s" s="1" r="C29">
+      <c r="E29" s="1" t="s">
         <v>69</v>
       </c>
-      <c t="s" s="1" r="E29">
+    </row>
+    <row r="30" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="30">
-      <c t="s" s="1" r="A30">
+      <c r="C30" s="1" t="s">
         <v>71</v>
       </c>
-      <c t="s" s="1" r="C30">
+      <c r="E30" s="1" t="s">
         <v>72</v>
       </c>
-      <c t="s" s="1" r="E30">
+    </row>
+    <row r="31" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="31">
-      <c t="s" s="1" r="A31">
-        <v>8</v>
-      </c>
-      <c t="s" s="1" r="C31">
+      <c r="E31" s="1" t="s">
         <v>74</v>
       </c>
-      <c t="s" s="1" r="E31">
+    </row>
+    <row r="32" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="32">
-      <c t="s" s="1" r="A32">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33">
-      <c t="s" s="1" r="A33">
-        <v>39</v>
-      </c>
-      <c t="s" s="1" r="E33">
+      <c r="H33" s="1" t="s">
         <v>76</v>
       </c>
-      <c t="s" s="1" r="H33">
+      <c r="I33" s="1" t="s">
         <v>77</v>
       </c>
-      <c t="s" s="1" r="I33">
+    </row>
+    <row r="34" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="34">
-      <c t="s" s="3" r="A34">
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>79</v>
       </c>
-      <c s="1" r="E34"/>
-    </row>
-    <row r="35">
-      <c t="s" s="1" r="A35">
+      <c r="C35" t="s">
         <v>80</v>
-      </c>
-      <c t="s" r="C35">
-        <v>81</v>
       </c>
       <c r="D35">
         <v>10</v>
       </c>
-      <c s="1" r="E35"/>
-    </row>
-    <row r="36">
-      <c t="s" s="1" r="A36">
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
-      <c t="s" r="B36">
+      <c r="B36" t="s">
+        <v>81</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>82</v>
       </c>
-      <c t="s" s="1" r="E36">
+    </row>
+    <row r="37" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="37">
-      <c t="s" s="1" r="A37">
-        <v>39</v>
-      </c>
-      <c t="s" r="B37">
+      <c r="E37" s="1" t="s">
         <v>84</v>
       </c>
-      <c t="s" s="1" r="E37">
+    </row>
+    <row r="38" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="38">
-      <c t="s" s="1" r="A38">
-        <v>36</v>
-      </c>
-      <c t="s" r="B38">
+      <c r="C38" s="1" t="s">
         <v>86</v>
       </c>
-      <c t="s" s="1" r="C38">
+      <c r="E38" s="1" t="s">
         <v>87</v>
       </c>
-      <c t="s" s="1" r="E38">
+      <c r="J38" s="1" t="s">
         <v>88</v>
       </c>
-      <c t="s" s="1" r="J38">
+    </row>
+    <row r="39" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="39">
-      <c t="s" s="1" r="A39">
+      <c r="C39" s="1" t="s">
         <v>90</v>
       </c>
-      <c t="s" s="1" r="C39">
+      <c r="E39" s="1" t="s">
         <v>91</v>
       </c>
-      <c t="s" s="1" r="E39">
+      <c r="F39" t="s">
         <v>92</v>
-      </c>
-      <c t="s" r="F39">
-        <v>93</v>
       </c>
       <c r="G39">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="K39">
-        <v>94</v>
-      </c>
-      <c s="1" r="L39">
+      <c r="K39" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L39" s="1">
         <v>1</v>
       </c>
-      <c s="1" r="M39">
+      <c r="M39" s="1">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="9.14" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col max="1" min="1" customWidth="1" width="21.43"/>
-    <col max="2" min="2" customWidth="1" width="49.43"/>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="2" max="2" width="49.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2">
-      <c t="s" s="1" r="A2">
+      <c r="B2" s="1" t="s">
         <v>96</v>
       </c>
-      <c t="s" s="1" r="B2">
-        <v>97</v>
-      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="11.57" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col max="2" min="2" customWidth="1" width="18.14"/>
-    <col max="3" min="3" customWidth="1" width="15.86"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>98</v>
       </c>
-      <c t="s" s="1" r="B1">
-        <v>2</v>
-      </c>
-      <c t="s" s="1" r="C1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c t="s" s="1" r="A2">
+      <c r="B2" s="1" t="s">
         <v>99</v>
       </c>
-      <c t="s" s="1" r="B2">
+      <c r="C2" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>100</v>
       </c>
-      <c t="s" s="1" r="C2">
+      <c r="C3" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3">
-      <c t="s" s="1" r="A3">
-        <v>99</v>
-      </c>
-      <c t="s" s="1" r="B3">
+    <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>101</v>
       </c>
-      <c t="s" s="1" r="C3">
+      <c r="B4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4">
-      <c t="s" s="1" r="A4">
-        <v>102</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>103</v>
-      </c>
-      <c t="s" s="1" r="C4">
+      <c r="B5" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="5">
-      <c t="s" s="1" r="A5">
-        <v>102</v>
-      </c>
-      <c t="s" s="1" r="B5">
+      <c r="C5" s="1" t="s">
         <v>105</v>
       </c>
-      <c t="s" s="1" r="C5">
+    </row>
+    <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="6">
-      <c t="s" s="1" r="A6">
-        <v>102</v>
-      </c>
-      <c t="s" s="1" r="B6">
+      <c r="C6" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>107</v>
       </c>
-      <c t="s" s="1" r="C6">
+      <c r="C7" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7">
-      <c t="s" s="1" r="A7">
-        <v>102</v>
-      </c>
-      <c t="s" s="1" r="B7">
+    <row r="8" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>108</v>
       </c>
-      <c t="s" s="1" r="C7">
+      <c r="C8" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8">
-      <c t="s" s="1" r="A8">
-        <v>102</v>
-      </c>
-      <c t="s" s="1" r="B8">
+    <row r="9" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>109</v>
       </c>
-      <c t="s" s="1" r="C8">
+      <c r="C9" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9">
-      <c t="s" s="1" r="A9">
-        <v>102</v>
-      </c>
-      <c t="s" s="1" r="B9">
+    <row r="10" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>110</v>
       </c>
-      <c t="s" s="1" r="C9">
+      <c r="C10" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="10">
-      <c t="s" s="1" r="A10">
-        <v>102</v>
-      </c>
-      <c t="s" s="1" r="B10">
+    <row r="11" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
         <v>111</v>
       </c>
-      <c t="s" s="1" r="C10">
+      <c r="C12" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="11">
-      <c t="s" r="A11">
+    <row r="13" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B11">
-        <v>20</v>
-      </c>
-      <c t="s" r="C11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12">
-      <c t="s" r="A12">
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B12">
-        <v>112</v>
-      </c>
-      <c t="s" r="C12">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13">
-      <c t="s" r="A13">
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B13">
-        <v>113</v>
-      </c>
-      <c t="s" r="C13">
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="14">
-      <c t="s" r="A14">
+      <c r="C16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B14">
-        <v>51</v>
-      </c>
-      <c t="s" r="C14">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15">
-      <c t="s" r="A15">
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B15">
-        <v>54</v>
-      </c>
-      <c t="s" r="C15">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16">
-      <c t="s" r="A16">
+      <c r="B18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c t="s" r="B16">
-        <v>115</v>
-      </c>
-      <c t="s" r="C16">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17">
-      <c t="s" r="A17">
-        <v>15</v>
-      </c>
-      <c t="s" r="B17">
-        <v>116</v>
-      </c>
-      <c t="s" r="C17">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18">
-      <c t="s" r="A18">
-        <v>15</v>
-      </c>
-      <c t="s" r="B18">
-        <v>118</v>
-      </c>
-      <c t="s" r="C18">
+      <c r="B19" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="19">
-      <c t="s" r="A19">
-        <v>15</v>
-      </c>
-      <c t="s" r="B19">
-        <v>120</v>
-      </c>
-      <c t="s" r="C19">
-        <v>120</v>
+      <c r="C19" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="11.57" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col max="2" min="2" customWidth="1" width="13.57"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>121</v>
       </c>
-      <c t="s" s="1" r="B1">
+    </row>
+    <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="2">
-      <c t="s" s="1" r="A2">
+      <c r="B2" s="1" t="s">
         <v>123</v>
       </c>
-      <c t="s" s="1" r="B2">
+    </row>
+    <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="3">
-      <c t="s" s="1" r="A3">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
-      <c s="1" r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c t="s" s="1" r="A4">
+      <c r="B4" s="1" t="s">
         <v>126</v>
       </c>
-      <c t="s" s="1" r="B4">
-        <v>127</v>
-      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated example form definition and generation.
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -139,9 +139,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>Hello {{name.value}}</t>
-  </si>
-  <si>
     <t>label dynamic_label_end</t>
   </si>
   <si>
@@ -271,9 +268,6 @@
     <t>data('x') === 10</t>
   </si>
   <si>
-    <t>x = {{x.value}}</t>
-  </si>
-  <si>
     <t>selected(data('examples'), 'custom_template')</t>
   </si>
   <si>
@@ -401,6 +395,12 @@
   </si>
   <si>
     <t>select_multiple continents</t>
+  </si>
+  <si>
+    <t>Hello {{name}}</t>
+  </si>
+  <si>
+    <t>x = {{x}}</t>
   </si>
 </sst>
 </file>
@@ -782,7 +782,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -964,32 +964,32 @@
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>40</v>
+      <c r="E14" s="5" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
         <v>44</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -997,71 +997,71 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
         <v>54</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
         <v>58</v>
-      </c>
-      <c r="B23" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
@@ -1069,31 +1069,31 @@
         <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" t="s">
         <v>66</v>
-      </c>
-      <c r="B27" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
@@ -1101,21 +1101,21 @@
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
@@ -1123,15 +1123,15 @@
         <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
@@ -1139,27 +1139,27 @@
         <v>39</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" t="s">
         <v>79</v>
-      </c>
-      <c r="C35" t="s">
-        <v>80</v>
       </c>
       <c r="D35">
         <v>10</v>
@@ -1171,10 +1171,10 @@
         <v>39</v>
       </c>
       <c r="B36" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
@@ -1182,10 +1182,10 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
@@ -1193,36 +1193,36 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="F39" t="s">
         <v>90</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F39" t="s">
-        <v>92</v>
       </c>
       <c r="G39">
         <v>5</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L39" s="1">
         <v>1</v>
@@ -1253,15 +1253,15 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1283,7 +1283,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1294,101 +1294,101 @@
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1407,10 +1407,10 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1418,10 +1418,10 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1429,10 +1429,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1440,10 +1440,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1451,10 +1451,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1462,10 +1462,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1473,10 +1473,10 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1484,10 +1484,10 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1508,23 +1508,23 @@
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -1532,10 +1532,10 @@
     </row>
     <row r="4" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on adding csv support
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet name="survey" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="calculates" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="choices" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="settings" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet sheetId="1" name="survey" state="visible" r:id="rId3"/>
+    <sheet sheetId="2" name="calculates" state="visible" r:id="rId4"/>
+    <sheet sheetId="3" name="choices" state="visible" r:id="rId5"/>
+    <sheet sheetId="4" name="settings" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="128" count="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="132">
   <si>
     <t>type</t>
   </si>
@@ -25,9 +25,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>assign</t>
-  </si>
-  <si>
     <t>label</t>
   </si>
   <si>
@@ -124,6 +121,9 @@
     <t>not(selected(data('examples'), 'dynamic_label'))</t>
   </si>
   <si>
+    <t>begin screen</t>
+  </si>
+  <si>
     <t>text</t>
   </si>
   <si>
@@ -139,6 +139,27 @@
     <t>Hello {{name.value}}</t>
   </si>
   <si>
+    <t>end screen</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>avg_coffee</t>
+  </si>
+  <si>
+    <t>On average, how many cups of coffee do you drink in a day?</t>
+  </si>
+  <si>
+    <t>coffee_today</t>
+  </si>
+  <si>
+    <t>How many cups of coffee did you drink today?</t>
+  </si>
+  <si>
+    <t>data('avg_coffee')</t>
+  </si>
+  <si>
     <t>label dynamic_label_end</t>
   </si>
   <si>
@@ -190,13 +211,10 @@
     <t>Record your location:</t>
   </si>
   <si>
-    <t>begin screen</t>
-  </si>
-  <si>
     <t>selected(data('examples'), 'screen_group')</t>
   </si>
   <si>
-    <t>select continents</t>
+    <t>select_multiple continents</t>
   </si>
   <si>
     <t>visited_continents</t>
@@ -214,9 +232,6 @@
     <t>Have you visited Seattle?</t>
   </si>
   <si>
-    <t>end screen</t>
-  </si>
-  <si>
     <t>goto media_end</t>
   </si>
   <si>
@@ -284,9 +299,6 @@
   </si>
   <si>
     <t>test.handlebars</t>
-  </si>
-  <si>
-    <t>integer</t>
   </si>
   <si>
     <t>rating</t>
@@ -480,18 +492,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" xfId="0" fontId="0" fillId="2" borderId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="1"/>
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="2" fillId="3" borderId="0" applyFill="1"/>
-    <xf numFmtId="0" applyFont="1" xfId="0" fontId="3" fillId="4" borderId="0" applyFill="1"/>
+    <xf fillId="3" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="2" applyFill="1"/>
+    <xf fillId="4" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="3" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -504,21 +516,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="11.57" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.57" defaultRowHeight="12.75"/>
   <cols>
-    <col max="1" min="1" customWidth="1" width="27.14"/>
-    <col max="2" min="2" customWidth="1" width="45.86"/>
-    <col max="3" min="3" customWidth="1" width="24.86"/>
-    <col max="4" min="4" customWidth="1" width="19.14"/>
-    <col max="5" min="5" customWidth="1" width="41.86"/>
-    <col max="6" min="6" customWidth="1" width="40.0"/>
-    <col max="8" min="8" customWidth="1" width="20.57"/>
-    <col max="9" min="9" customWidth="1" width="13.0"/>
-    <col max="10" min="10" customWidth="1" width="15.86"/>
-    <col max="11" min="11" customWidth="1" width="18.29"/>
-    <col max="12" min="12" customWidth="1" width="18.43"/>
-    <col max="13" min="13" customWidth="1" width="19.0"/>
-    <col max="14" min="14" customWidth="1" width="27.0"/>
+    <col min="1" customWidth="1" max="1" width="27.14"/>
+    <col min="2" customWidth="1" max="2" width="40.86"/>
+    <col min="3" customWidth="1" max="3" width="24.86"/>
+    <col min="4" customWidth="1" max="4" width="41.86"/>
+    <col min="5" customWidth="1" max="5" width="40.0"/>
+    <col min="6" customWidth="1" max="6" width="14.29"/>
+    <col min="7" customWidth="1" max="7" width="20.57"/>
+    <col min="8" customWidth="1" max="8" width="13.0"/>
+    <col min="9" customWidth="1" max="9" width="15.86"/>
+    <col min="10" customWidth="1" max="10" width="18.29"/>
+    <col min="11" customWidth="1" max="11" width="18.43"/>
+    <col min="12" customWidth="1" max="12" width="19.0"/>
+    <col min="13" customWidth="1" max="13" width="27.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -561,392 +573,421 @@
       <c t="s" s="1" r="M1">
         <v>12</v>
       </c>
-      <c t="s" s="1" r="N1">
+    </row>
+    <row customHeight="1" r="2" ht="18.0">
+      <c t="s" s="1" r="A2">
         <v>13</v>
       </c>
-    </row>
-    <row ht="18.0" r="2" customHeight="1">
-      <c t="s" s="1" r="A2">
+      <c t="s" r="C2">
         <v>14</v>
       </c>
-      <c t="s" r="C2">
+      <c t="s" r="D2">
         <v>15</v>
-      </c>
-      <c t="s" r="E2">
-        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="2" r="A3">
+        <v>16</v>
+      </c>
+      <c t="s" s="1" r="B3">
         <v>17</v>
-      </c>
-      <c t="s" s="1" r="B3">
-        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
+        <v>18</v>
+      </c>
+      <c t="s" r="C4">
         <v>19</v>
       </c>
-      <c t="s" r="C4">
+      <c t="s" r="D4">
         <v>20</v>
       </c>
       <c t="s" r="E4">
         <v>21</v>
       </c>
-      <c t="s" r="F4">
-        <v>22</v>
-      </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c t="s" r="B5">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="3" r="A6">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="2" r="A7">
+        <v>24</v>
+      </c>
+      <c t="s" s="1" r="B7">
         <v>25</v>
-      </c>
-      <c t="s" s="1" r="B7">
-        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c t="s" r="A8">
+        <v>26</v>
+      </c>
+      <c t="s" r="C8">
+        <v>26</v>
+      </c>
+      <c t="s" r="D8">
         <v>27</v>
-      </c>
-      <c t="s" r="C8">
-        <v>27</v>
-      </c>
-      <c t="s" r="E8">
-        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c t="s" r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c t="s" r="C9">
+        <v>28</v>
+      </c>
+      <c t="s" r="D9">
         <v>29</v>
-      </c>
-      <c t="s" r="E9">
-        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c t="s" r="A10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c t="s" r="C10">
+        <v>30</v>
+      </c>
+      <c t="s" r="D10">
         <v>31</v>
-      </c>
-      <c t="s" r="E10">
-        <v>32</v>
       </c>
     </row>
     <row r="11">
       <c t="s" s="3" r="A11">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="2" r="A12">
+        <v>33</v>
+      </c>
+      <c t="s" s="1" r="B12">
         <v>34</v>
       </c>
-      <c t="s" s="1" r="B12">
+    </row>
+    <row r="13">
+      <c t="s" r="A13">
         <v>35</v>
-      </c>
-    </row>
-    <row r="13">
-      <c t="s" s="1" r="A13">
-        <v>36</v>
-      </c>
-      <c t="s" s="1" r="C13">
-        <v>2</v>
-      </c>
-      <c t="s" s="1" r="E13">
-        <v>37</v>
-      </c>
-      <c t="s" s="1" r="F13">
-        <v>38</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
+        <v>36</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>2</v>
+      </c>
+      <c t="s" s="1" r="D14">
+        <v>37</v>
+      </c>
+      <c t="s" s="1" r="E14">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" s="1" r="A15">
         <v>39</v>
       </c>
-      <c t="s" s="1" r="E14">
+      <c t="s" s="1" r="D15">
         <v>40</v>
       </c>
     </row>
-    <row ht="18.0" r="15" customHeight="1">
-      <c t="s" s="3" r="A15">
+    <row r="16">
+      <c t="s" s="1" r="A16">
         <v>41</v>
       </c>
     </row>
-    <row ht="18.0" r="16" customHeight="1">
-      <c t="s" s="2" r="A16">
+    <row r="17">
+      <c t="s" s="1" r="A17">
         <v>42</v>
       </c>
-      <c t="s" s="1" r="B16">
+      <c t="s" r="C17">
         <v>43</v>
       </c>
-    </row>
-    <row ht="18.0" r="17" customHeight="1">
-      <c t="s" s="1" r="A17">
+      <c t="s" r="D17">
         <v>44</v>
       </c>
-      <c t="s" r="C17">
+    </row>
+    <row r="18">
+      <c t="s" s="1" r="A18">
+        <v>42</v>
+      </c>
+      <c t="s" r="C18">
         <v>45</v>
       </c>
-      <c t="s" s="1" r="E17">
+      <c t="s" r="D18">
         <v>46</v>
       </c>
-    </row>
-    <row ht="18.0" r="18" customHeight="1">
-      <c t="s" s="1" r="A18">
+      <c t="s" r="F18">
+        <v>47</v>
+      </c>
+    </row>
+    <row customHeight="1" r="19" ht="18.0">
+      <c t="s" s="3" r="A19">
+        <v>48</v>
+      </c>
+    </row>
+    <row customHeight="1" r="20" ht="18.0">
+      <c t="s" s="2" r="A20">
+        <v>49</v>
+      </c>
+      <c t="s" s="1" r="B20">
+        <v>50</v>
+      </c>
+    </row>
+    <row customHeight="1" r="21" ht="18.0">
+      <c t="s" s="1" r="A21">
+        <v>51</v>
+      </c>
+      <c t="s" r="C21">
+        <v>52</v>
+      </c>
+      <c t="s" s="1" r="D21">
+        <v>53</v>
+      </c>
+    </row>
+    <row customHeight="1" r="22" ht="18.0">
+      <c t="s" s="1" r="A22">
         <v>39</v>
       </c>
-      <c t="s" r="B18">
-        <v>47</v>
-      </c>
-      <c t="s" s="1" r="E18">
-        <v>48</v>
-      </c>
-    </row>
-    <row ht="18.0" r="19" customHeight="1">
-      <c t="s" s="1" r="A19">
-        <v>49</v>
-      </c>
-      <c t="s" r="C19">
-        <v>49</v>
-      </c>
-      <c t="s" s="1" r="E19">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20">
-      <c t="s" s="1" r="A20">
-        <v>51</v>
-      </c>
-      <c t="s" s="1" r="C20">
-        <v>51</v>
-      </c>
-      <c t="s" s="1" r="E20">
-        <v>52</v>
-      </c>
-    </row>
-    <row ht="18.0" r="21" customHeight="1">
-      <c t="s" s="3" r="A21">
-        <v>53</v>
-      </c>
-      <c s="1" r="C21"/>
-    </row>
-    <row ht="18.0" r="22" customHeight="1">
-      <c t="s" s="1" r="A22">
+      <c t="s" r="B22">
         <v>54</v>
       </c>
-      <c t="s" r="B22">
+      <c t="s" s="1" r="D22">
         <v>55</v>
       </c>
-      <c t="s" s="1" r="C22">
+    </row>
+    <row customHeight="1" r="23" ht="18.0">
+      <c t="s" s="1" r="A23">
         <v>56</v>
       </c>
-      <c t="s" s="1" r="E22">
+      <c t="s" r="C23">
+        <v>56</v>
+      </c>
+      <c t="s" s="1" r="D23">
         <v>57</v>
-      </c>
-    </row>
-    <row r="23">
-      <c t="s" s="1" r="A23">
-        <v>58</v>
-      </c>
-      <c t="s" r="B23">
-        <v>59</v>
       </c>
     </row>
     <row r="24">
       <c t="s" s="1" r="A24">
+        <v>58</v>
+      </c>
+      <c t="s" s="1" r="C24">
+        <v>58</v>
+      </c>
+      <c t="s" s="1" r="D24">
+        <v>59</v>
+      </c>
+    </row>
+    <row customHeight="1" r="25" ht="18.0">
+      <c t="s" s="3" r="A25">
         <v>60</v>
       </c>
-      <c t="s" s="1" r="C24">
+      <c s="1" r="C25"/>
+    </row>
+    <row customHeight="1" r="26" ht="18.0">
+      <c t="s" s="1" r="A26">
         <v>61</v>
       </c>
-      <c t="s" s="1" r="E24">
+      <c t="s" r="B26">
         <v>62</v>
       </c>
-    </row>
-    <row r="25">
-      <c t="s" s="1" r="A25">
-        <v>19</v>
-      </c>
-      <c t="s" s="1" r="B25">
+      <c t="s" s="1" r="C26">
         <v>63</v>
       </c>
-      <c t="s" s="1" r="C25">
+      <c t="s" s="1" r="D26">
         <v>64</v>
       </c>
-      <c t="s" s="1" r="E25">
+    </row>
+    <row r="27">
+      <c t="s" s="1" r="A27">
+        <v>35</v>
+      </c>
+      <c t="s" r="B27">
         <v>65</v>
-      </c>
-    </row>
-    <row r="26">
-      <c t="s" s="1" r="A26">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27">
-      <c t="s" s="4" r="A27">
-        <v>67</v>
-      </c>
-      <c t="s" r="B27">
-        <v>68</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
-        <v>58</v>
+        <v>66</v>
+      </c>
+      <c t="s" s="1" r="C28">
+        <v>67</v>
+      </c>
+      <c t="s" s="1" r="D28">
+        <v>68</v>
       </c>
     </row>
     <row r="29">
       <c t="s" s="1" r="A29">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c t="s" s="1" r="B29">
+        <v>69</v>
       </c>
       <c t="s" s="1" r="C29">
-        <v>69</v>
-      </c>
-      <c t="s" s="1" r="E29">
         <v>70</v>
+      </c>
+      <c t="s" s="1" r="D29">
+        <v>71</v>
       </c>
     </row>
     <row r="30">
       <c t="s" s="1" r="A30">
-        <v>71</v>
-      </c>
-      <c t="s" s="1" r="C30">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31">
+      <c t="s" s="4" r="A31">
         <v>72</v>
       </c>
-      <c t="s" s="1" r="E30">
+      <c t="s" r="B31">
         <v>73</v>
-      </c>
-    </row>
-    <row r="31">
-      <c t="s" s="1" r="A31">
-        <v>8</v>
-      </c>
-      <c t="s" s="1" r="C31">
-        <v>74</v>
-      </c>
-      <c t="s" s="1" r="E31">
-        <v>75</v>
       </c>
     </row>
     <row r="32">
       <c t="s" s="1" r="A32">
-        <v>66</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>39</v>
-      </c>
-      <c t="s" s="1" r="E33">
+        <v>6</v>
+      </c>
+      <c t="s" s="1" r="C33">
+        <v>74</v>
+      </c>
+      <c t="s" s="1" r="D33">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34">
+      <c t="s" s="1" r="A34">
         <v>76</v>
       </c>
-      <c t="s" s="1" r="H33">
+      <c t="s" s="1" r="C34">
         <v>77</v>
       </c>
-      <c t="s" s="1" r="I33">
+      <c t="s" s="1" r="D34">
         <v>78</v>
       </c>
-    </row>
-    <row r="34">
-      <c t="s" s="3" r="A34">
-        <v>79</v>
-      </c>
-      <c s="1" r="E34"/>
     </row>
     <row r="35">
       <c t="s" s="1" r="A35">
+        <v>7</v>
+      </c>
+      <c t="s" s="1" r="C35">
+        <v>79</v>
+      </c>
+      <c t="s" s="1" r="D35">
         <v>80</v>
       </c>
-      <c t="s" r="C35">
-        <v>81</v>
-      </c>
-      <c r="D35">
-        <v>10</v>
-      </c>
-      <c s="1" r="E35"/>
     </row>
     <row r="36">
       <c t="s" s="1" r="A36">
-        <v>39</v>
-      </c>
-      <c t="s" r="B36">
-        <v>82</v>
-      </c>
-      <c t="s" s="1" r="E36">
-        <v>83</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37">
       <c t="s" s="1" r="A37">
         <v>39</v>
       </c>
-      <c t="s" r="B37">
+      <c t="s" s="1" r="D37">
+        <v>81</v>
+      </c>
+      <c t="s" s="1" r="G37">
+        <v>82</v>
+      </c>
+      <c t="s" s="1" r="H37">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38">
+      <c t="s" s="3" r="A38">
         <v>84</v>
       </c>
-      <c t="s" s="1" r="E37">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38">
-      <c t="s" s="1" r="A38">
-        <v>36</v>
-      </c>
-      <c t="s" r="B38">
-        <v>86</v>
-      </c>
-      <c t="s" s="1" r="C38">
-        <v>87</v>
-      </c>
-      <c t="s" s="1" r="E38">
-        <v>88</v>
-      </c>
-      <c t="s" s="1" r="J38">
-        <v>89</v>
-      </c>
+      <c s="1" r="D38"/>
     </row>
     <row r="39">
       <c t="s" s="1" r="A39">
+        <v>85</v>
+      </c>
+      <c t="s" r="C39">
+        <v>86</v>
+      </c>
+      <c s="1" r="D39"/>
+    </row>
+    <row r="40">
+      <c t="s" s="1" r="A40">
+        <v>39</v>
+      </c>
+      <c t="s" r="B40">
+        <v>87</v>
+      </c>
+      <c t="s" s="1" r="D40">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41">
+      <c t="s" s="1" r="A41">
+        <v>39</v>
+      </c>
+      <c t="s" r="B41">
+        <v>89</v>
+      </c>
+      <c t="s" s="1" r="D41">
         <v>90</v>
       </c>
-      <c t="s" s="1" r="C39">
+    </row>
+    <row r="42">
+      <c t="s" s="1" r="A42">
+        <v>36</v>
+      </c>
+      <c t="s" r="B42">
         <v>91</v>
       </c>
-      <c t="s" s="1" r="E39">
+      <c t="s" s="1" r="C42">
         <v>92</v>
       </c>
-      <c t="s" r="F39">
+      <c t="s" s="1" r="D42">
         <v>93</v>
       </c>
-      <c r="G39">
+      <c t="s" s="1" r="I42">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43">
+      <c t="s" s="1" r="A43">
+        <v>42</v>
+      </c>
+      <c t="s" s="1" r="C43">
+        <v>95</v>
+      </c>
+      <c t="s" s="1" r="D43">
+        <v>96</v>
+      </c>
+      <c t="s" r="E43">
+        <v>97</v>
+      </c>
+      <c r="F43">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="K39">
-        <v>94</v>
-      </c>
-      <c s="1" r="L39">
+      <c t="s" s="1" r="J43">
+        <v>98</v>
+      </c>
+      <c s="1" r="K43">
         <v>1</v>
       </c>
-      <c s="1" r="M39">
+      <c s="1" r="L43">
         <v>10</v>
       </c>
     </row>
@@ -959,10 +1000,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="9.14" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="9.14" defaultRowHeight="12.75"/>
   <cols>
-    <col max="1" min="1" customWidth="1" width="21.43"/>
-    <col max="2" min="2" customWidth="1" width="49.43"/>
+    <col min="1" customWidth="1" max="1" width="21.43"/>
+    <col min="2" customWidth="1" max="2" width="49.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -970,15 +1011,15 @@
         <v>2</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -990,219 +1031,219 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="11.57" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.57" defaultRowHeight="12.75"/>
   <cols>
-    <col max="2" min="2" customWidth="1" width="18.14"/>
-    <col max="3" min="3" customWidth="1" width="15.86"/>
+    <col min="2" customWidth="1" max="2" width="18.14"/>
+    <col min="3" customWidth="1" max="3" width="15.86"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c t="s" s="1" r="B1">
         <v>2</v>
       </c>
       <c t="s" s="1" r="C1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B6">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B9">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11">
       <c t="s" r="A11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c t="s" r="B11">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c t="s" r="C11">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c t="s" r="A12">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c t="s" r="B12">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c t="s" r="C12">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13">
       <c t="s" r="A13">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c t="s" r="B13">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c t="s" r="C13">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14">
       <c t="s" r="A14">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c t="s" r="B14">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c t="s" r="C14">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15">
       <c t="s" r="A15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c t="s" r="B15">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c t="s" r="C15">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16">
       <c t="s" r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c t="s" r="B16">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c t="s" r="C16">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17">
       <c t="s" r="A17">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c t="s" r="B17">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c t="s" r="C17">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18">
       <c t="s" r="A18">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c t="s" r="B18">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c t="s" r="C18">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19">
       <c t="s" r="A19">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c t="s" r="B19">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c t="s" r="C19">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1214,30 +1255,30 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" defaultColWidth="11.57" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.57" defaultRowHeight="12.75"/>
   <cols>
-    <col max="2" min="2" customWidth="1" width="13.57"/>
+    <col min="2" customWidth="1" max="2" width="13.57"/>
   </cols>
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c s="1" r="B3">
         <v>1</v>
@@ -1245,10 +1286,10 @@
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing some issues with csv cascading select example and dropdowns
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="132">
   <si>
     <t>type</t>
   </si>
@@ -121,115 +121,115 @@
     <t>not(selected(data('examples'), 'dynamic_label'))</t>
   </si>
   <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Enter your name</t>
+  </si>
+  <si>
+    <t>Please use your full name</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>{{#if name}}Hello {{name}}{{/if}}</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>avg_coffee</t>
+  </si>
+  <si>
+    <t>On average, how many cups of coffee do you drink in a day?</t>
+  </si>
+  <si>
+    <t>coffee_today</t>
+  </si>
+  <si>
+    <t>How many cups of coffee did you drink today?</t>
+  </si>
+  <si>
+    <t>data('avg_coffee')</t>
+  </si>
+  <si>
+    <t>label dynamic_label_end</t>
+  </si>
+  <si>
+    <t>goto datetime_end</t>
+  </si>
+  <si>
+    <t>not(selected(data('examples'), 'datetime'))</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>born</t>
+  </si>
+  <si>
+    <t>When were you born?</t>
+  </si>
+  <si>
+    <t>data('born').getDay() === now().getDay() &amp;&amp; data('born').getMonth() === now().getMonth()</t>
+  </si>
+  <si>
+    <t>Happy Birthday!</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>What time is it?</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>When will you be available for a follow up survey?</t>
+  </si>
+  <si>
+    <t>label datetime_end</t>
+  </si>
+  <si>
+    <t>geopoint</t>
+  </si>
+  <si>
+    <t>selected(data('examples'), 'geopoint')</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Record your location:</t>
+  </si>
+  <si>
     <t>begin screen</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>Enter your name</t>
-  </si>
-  <si>
-    <t>Please use your full name</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>{{#if name}}Hello {{name}}{{/if}}</t>
+    <t>selected(data('examples'), 'screen_group')</t>
+  </si>
+  <si>
+    <t>select_multiple continents</t>
+  </si>
+  <si>
+    <t>visited_continents</t>
+  </si>
+  <si>
+    <t>Which continents have you visited?</t>
+  </si>
+  <si>
+    <t>calculates.ask_about_seattle()</t>
+  </si>
+  <si>
+    <t>visited_seattle</t>
+  </si>
+  <si>
+    <t>Have you visited Seattle?</t>
   </si>
   <si>
     <t>end screen</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>avg_coffee</t>
-  </si>
-  <si>
-    <t>On average, how many cups of coffee do you drink in a day?</t>
-  </si>
-  <si>
-    <t>coffee_today</t>
-  </si>
-  <si>
-    <t>How many cups of coffee did you drink today?</t>
-  </si>
-  <si>
-    <t>data('avg_coffee')</t>
-  </si>
-  <si>
-    <t>label dynamic_label_end</t>
-  </si>
-  <si>
-    <t>goto datetime_end</t>
-  </si>
-  <si>
-    <t>not(selected(data('examples'), 'datetime'))</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>born</t>
-  </si>
-  <si>
-    <t>When were you born?</t>
-  </si>
-  <si>
-    <t>data('born').getDay() === now().getDay() &amp;&amp; data('born').getMonth() === now().getMonth()</t>
-  </si>
-  <si>
-    <t>Happy Birthday!</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>What time is it?</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>When will you be available for a follow up survey?</t>
-  </si>
-  <si>
-    <t>label datetime_end</t>
-  </si>
-  <si>
-    <t>geopoint</t>
-  </si>
-  <si>
-    <t>selected(data('examples'), 'geopoint')</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>Record your location:</t>
-  </si>
-  <si>
-    <t>selected(data('examples'), 'screen_group')</t>
-  </si>
-  <si>
-    <t>select_multiple continents</t>
-  </si>
-  <si>
-    <t>visited_continents</t>
-  </si>
-  <si>
-    <t>Which continents have you visited?</t>
-  </si>
-  <si>
-    <t>calculates.ask_about_seattle()</t>
-  </si>
-  <si>
-    <t>visited_seattle</t>
-  </si>
-  <si>
-    <t>Have you visited Seattle?</t>
   </si>
   <si>
     <t>goto media_end</t>
@@ -675,319 +675,309 @@
       </c>
     </row>
     <row r="13">
-      <c t="s" r="A13">
+      <c t="s" s="1" r="A13">
         <v>35</v>
+      </c>
+      <c t="s" s="1" r="C13">
+        <v>2</v>
+      </c>
+      <c t="s" s="1" r="D13">
+        <v>36</v>
+      </c>
+      <c t="s" s="1" r="E13">
+        <v>37</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>36</v>
-      </c>
-      <c t="s" s="1" r="C14">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c t="s" s="1" r="D14">
-        <v>37</v>
-      </c>
-      <c t="s" s="1" r="E14">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>39</v>
-      </c>
-      <c t="s" s="1" r="D15">
         <v>40</v>
+      </c>
+      <c t="s" r="C15">
+        <v>41</v>
+      </c>
+      <c t="s" r="D15">
+        <v>42</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17">
-      <c t="s" s="1" r="A17">
-        <v>42</v>
-      </c>
-      <c t="s" r="C17">
+        <v>40</v>
+      </c>
+      <c t="s" r="C16">
         <v>43</v>
       </c>
-      <c t="s" r="D17">
+      <c t="s" r="D16">
         <v>44</v>
       </c>
-    </row>
-    <row r="18">
-      <c t="s" s="1" r="A18">
-        <v>42</v>
-      </c>
-      <c t="s" r="C18">
+      <c t="s" r="F16">
         <v>45</v>
       </c>
-      <c t="s" r="D18">
+    </row>
+    <row customHeight="1" r="17" ht="18.0">
+      <c t="s" s="3" r="A17">
         <v>46</v>
       </c>
-      <c t="s" r="F18">
+    </row>
+    <row customHeight="1" r="18" ht="18.0">
+      <c t="s" s="2" r="A18">
         <v>47</v>
       </c>
+      <c t="s" s="1" r="B18">
+        <v>48</v>
+      </c>
     </row>
     <row customHeight="1" r="19" ht="18.0">
-      <c t="s" s="3" r="A19">
-        <v>48</v>
+      <c t="s" s="1" r="A19">
+        <v>49</v>
+      </c>
+      <c t="s" r="C19">
+        <v>50</v>
+      </c>
+      <c t="s" s="1" r="D19">
+        <v>51</v>
       </c>
     </row>
     <row customHeight="1" r="20" ht="18.0">
-      <c t="s" s="2" r="A20">
-        <v>49</v>
-      </c>
-      <c t="s" s="1" r="B20">
-        <v>50</v>
+      <c t="s" s="1" r="A20">
+        <v>38</v>
+      </c>
+      <c t="s" r="B20">
+        <v>52</v>
+      </c>
+      <c t="s" s="1" r="D20">
+        <v>53</v>
       </c>
     </row>
     <row customHeight="1" r="21" ht="18.0">
       <c t="s" s="1" r="A21">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c t="s" r="C21">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c t="s" s="1" r="D21">
-        <v>53</v>
-      </c>
-    </row>
-    <row customHeight="1" r="22" ht="18.0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22">
       <c t="s" s="1" r="A22">
-        <v>39</v>
-      </c>
-      <c t="s" r="B22">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c t="s" s="1" r="C22">
+        <v>56</v>
       </c>
       <c t="s" s="1" r="D22">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row customHeight="1" r="23" ht="18.0">
-      <c t="s" s="1" r="A23">
-        <v>56</v>
-      </c>
-      <c t="s" r="C23">
-        <v>56</v>
-      </c>
-      <c t="s" s="1" r="D23">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24">
+      <c t="s" s="3" r="A23">
+        <v>58</v>
+      </c>
+      <c s="1" r="C23"/>
+    </row>
+    <row customHeight="1" r="24" ht="18.0">
       <c t="s" s="1" r="A24">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c t="s" r="B24">
+        <v>60</v>
       </c>
       <c t="s" s="1" r="C24">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c t="s" s="1" r="D24">
-        <v>59</v>
-      </c>
-    </row>
-    <row customHeight="1" r="25" ht="18.0">
-      <c t="s" s="3" r="A25">
-        <v>60</v>
-      </c>
-      <c s="1" r="C25"/>
-    </row>
-    <row customHeight="1" r="26" ht="18.0">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25">
+      <c t="s" s="1" r="A25">
+        <v>63</v>
+      </c>
+      <c t="s" r="B25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26">
       <c t="s" s="1" r="A26">
-        <v>61</v>
-      </c>
-      <c t="s" r="B26">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c t="s" s="1" r="C26">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c t="s" s="1" r="D26">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27">
       <c t="s" s="1" r="A27">
-        <v>35</v>
-      </c>
-      <c t="s" r="B27">
-        <v>65</v>
+        <v>18</v>
+      </c>
+      <c t="s" s="1" r="B27">
+        <v>68</v>
+      </c>
+      <c t="s" s="1" r="C27">
+        <v>69</v>
+      </c>
+      <c t="s" s="1" r="D27">
+        <v>70</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
-        <v>66</v>
-      </c>
-      <c t="s" s="1" r="C28">
-        <v>67</v>
-      </c>
-      <c t="s" s="1" r="D28">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29">
-      <c t="s" s="1" r="A29">
-        <v>18</v>
-      </c>
-      <c t="s" s="1" r="B29">
-        <v>69</v>
-      </c>
-      <c t="s" s="1" r="C29">
-        <v>70</v>
-      </c>
-      <c t="s" s="1" r="D29">
-        <v>71</v>
+      <c t="s" s="4" r="A29">
+        <v>72</v>
+      </c>
+      <c t="s" r="B29">
+        <v>73</v>
       </c>
     </row>
     <row r="30">
       <c t="s" s="1" r="A30">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31">
-      <c t="s" s="4" r="A31">
-        <v>72</v>
-      </c>
-      <c t="s" r="B31">
-        <v>73</v>
+      <c t="s" s="1" r="A31">
+        <v>6</v>
+      </c>
+      <c t="s" s="1" r="C31">
+        <v>74</v>
+      </c>
+      <c t="s" s="1" r="D31">
+        <v>75</v>
       </c>
     </row>
     <row r="32">
       <c t="s" s="1" r="A32">
-        <v>35</v>
+        <v>76</v>
+      </c>
+      <c t="s" s="1" r="C32">
+        <v>77</v>
+      </c>
+      <c t="s" s="1" r="D32">
+        <v>78</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c t="s" s="1" r="C33">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c t="s" s="1" r="D33">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34">
       <c t="s" s="1" r="A34">
-        <v>76</v>
-      </c>
-      <c t="s" s="1" r="C34">
-        <v>77</v>
-      </c>
-      <c t="s" s="1" r="D34">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35">
       <c t="s" s="1" r="A35">
-        <v>7</v>
-      </c>
-      <c t="s" s="1" r="C35">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c t="s" s="1" r="D35">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c t="s" s="1" r="G35">
+        <v>82</v>
+      </c>
+      <c t="s" s="1" r="H35">
+        <v>83</v>
       </c>
     </row>
     <row r="36">
-      <c t="s" s="1" r="A36">
-        <v>41</v>
-      </c>
+      <c t="s" s="3" r="A36">
+        <v>84</v>
+      </c>
+      <c s="1" r="D36"/>
     </row>
     <row r="37">
       <c t="s" s="1" r="A37">
-        <v>39</v>
-      </c>
-      <c t="s" s="1" r="D37">
-        <v>81</v>
-      </c>
-      <c t="s" s="1" r="G37">
-        <v>82</v>
-      </c>
-      <c t="s" s="1" r="H37">
-        <v>83</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c t="s" r="C37">
+        <v>86</v>
+      </c>
+      <c s="1" r="D37"/>
     </row>
     <row r="38">
-      <c t="s" s="3" r="A38">
-        <v>84</v>
-      </c>
-      <c s="1" r="D38"/>
+      <c t="s" s="1" r="A38">
+        <v>38</v>
+      </c>
+      <c t="s" r="B38">
+        <v>87</v>
+      </c>
+      <c t="s" s="1" r="D38">
+        <v>88</v>
+      </c>
     </row>
     <row r="39">
       <c t="s" s="1" r="A39">
-        <v>85</v>
-      </c>
-      <c t="s" r="C39">
-        <v>86</v>
-      </c>
-      <c s="1" r="D39"/>
+        <v>38</v>
+      </c>
+      <c t="s" r="B39">
+        <v>89</v>
+      </c>
+      <c t="s" s="1" r="D39">
+        <v>90</v>
+      </c>
     </row>
     <row r="40">
       <c t="s" s="1" r="A40">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c t="s" r="B40">
-        <v>87</v>
+        <v>91</v>
+      </c>
+      <c t="s" s="1" r="C40">
+        <v>92</v>
       </c>
       <c t="s" s="1" r="D40">
-        <v>88</v>
+        <v>93</v>
+      </c>
+      <c t="s" s="1" r="I40">
+        <v>94</v>
       </c>
     </row>
     <row r="41">
       <c t="s" s="1" r="A41">
-        <v>39</v>
-      </c>
-      <c t="s" r="B41">
-        <v>89</v>
+        <v>40</v>
+      </c>
+      <c t="s" s="1" r="C41">
+        <v>95</v>
       </c>
       <c t="s" s="1" r="D41">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42">
-      <c t="s" s="1" r="A42">
-        <v>36</v>
-      </c>
-      <c t="s" r="B42">
-        <v>91</v>
-      </c>
-      <c t="s" s="1" r="C42">
-        <v>92</v>
-      </c>
-      <c t="s" s="1" r="D42">
-        <v>93</v>
-      </c>
-      <c t="s" s="1" r="I42">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43">
-      <c t="s" s="1" r="A43">
-        <v>42</v>
-      </c>
-      <c t="s" s="1" r="C43">
-        <v>95</v>
-      </c>
-      <c t="s" s="1" r="D43">
         <v>96</v>
       </c>
-      <c t="s" r="E43">
+      <c t="s" r="E41">
         <v>97</v>
       </c>
-      <c r="F43">
+      <c r="F41">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="J43">
+      <c t="s" s="1" r="J41">
         <v>98</v>
       </c>
-      <c s="1" r="K43">
+      <c s="1" r="K41">
         <v>1</v>
       </c>
-      <c s="1" r="L43">
+      <c s="1" r="L41">
         <v>10</v>
       </c>
     </row>
@@ -1185,10 +1175,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B14">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c t="s" r="C14">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15">
@@ -1196,10 +1186,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B15">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c t="s" r="C15">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
Adding breathcounter and shared_table example forms
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="133">
   <si>
     <t>type</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>Scan a barcode</t>
+  </si>
+  <si>
+    <t>geopoint</t>
+  </si>
+  <si>
+    <t>Capture your location</t>
   </si>
   <si>
     <t>picture</t>
@@ -217,9 +223,6 @@
   </si>
   <si>
     <t>label datetime_end</t>
-  </si>
-  <si>
-    <t>geopoint</t>
   </si>
   <si>
     <t>selected(data('examples'), 'geopoint')</t>
@@ -658,7 +661,7 @@
     </row>
     <row r="9">
       <c t="s" r="A9">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c t="s" r="C9">
         <v>28</v>
@@ -669,7 +672,7 @@
     </row>
     <row r="10">
       <c t="s" r="A10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c t="s" r="C10">
         <v>30</v>
@@ -679,48 +682,48 @@
       </c>
     </row>
     <row r="11">
-      <c t="s" s="4" r="A11">
+      <c t="s" r="A11">
+        <v>6</v>
+      </c>
+      <c t="s" r="C11">
         <v>32</v>
       </c>
+      <c t="s" r="D11">
+        <v>33</v>
+      </c>
     </row>
     <row r="12">
-      <c t="s" s="2" r="A12">
-        <v>33</v>
-      </c>
-      <c t="s" s="1" r="B12">
+      <c t="s" s="4" r="A12">
         <v>34</v>
       </c>
     </row>
     <row r="13">
-      <c t="s" s="1" r="A13">
+      <c t="s" s="2" r="A13">
         <v>35</v>
       </c>
-      <c t="s" s="1" r="C13">
-        <v>2</v>
-      </c>
-      <c t="s" s="1" r="D13">
+      <c t="s" s="1" r="B13">
         <v>36</v>
-      </c>
-      <c t="s" s="1" r="E13">
-        <v>37</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
+        <v>37</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>2</v>
+      </c>
+      <c t="s" s="1" r="D14">
         <v>38</v>
       </c>
-      <c t="s" s="1" r="D14">
+      <c t="s" s="1" r="E14">
         <v>39</v>
-      </c>
-      <c t="s" r="E14">
-        <v>40</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>38</v>
-      </c>
-      <c t="s" r="D15">
+        <v>40</v>
+      </c>
+      <c t="s" s="1" r="D15">
         <v>41</v>
       </c>
       <c t="s" r="E15">
@@ -729,43 +732,40 @@
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>38</v>
-      </c>
-      <c t="s" s="3" r="D16">
+        <v>40</v>
+      </c>
+      <c t="s" r="D16">
         <v>43</v>
       </c>
-      <c t="s" s="1" r="G16">
+      <c t="s" r="E16">
         <v>44</v>
       </c>
-      <c t="s" s="1" r="H16">
+    </row>
+    <row r="17">
+      <c t="s" s="1" r="A17">
+        <v>40</v>
+      </c>
+      <c t="s" s="3" r="D17">
         <v>45</v>
       </c>
-    </row>
-    <row customHeight="1" r="17" ht="18.0">
-      <c t="s" s="4" r="A17">
+      <c t="s" s="1" r="G17">
         <v>46</v>
       </c>
-    </row>
-    <row r="18">
-      <c t="s" s="1" r="A18">
+      <c t="s" s="1" r="H17">
         <v>47</v>
       </c>
-      <c t="s" r="B18">
+    </row>
+    <row customHeight="1" r="18" ht="18.0">
+      <c t="s" s="4" r="A18">
         <v>48</v>
-      </c>
-      <c t="s" r="C18">
-        <v>49</v>
-      </c>
-      <c t="s" r="D18">
-        <v>50</v>
       </c>
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c t="s" r="B19">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c t="s" r="C19">
         <v>51</v>
@@ -773,34 +773,37 @@
       <c t="s" r="D19">
         <v>52</v>
       </c>
-      <c t="s" r="F19">
+    </row>
+    <row r="20">
+      <c t="s" s="1" r="A20">
+        <v>49</v>
+      </c>
+      <c t="s" r="B20">
+        <v>50</v>
+      </c>
+      <c t="s" r="C20">
         <v>53</v>
       </c>
-    </row>
-    <row customHeight="1" r="20" ht="18.0">
-      <c t="s" s="2" r="A20">
+      <c t="s" r="D20">
         <v>54</v>
       </c>
-      <c t="s" s="1" r="B20">
+      <c t="s" r="F20">
         <v>55</v>
       </c>
     </row>
     <row customHeight="1" r="21" ht="18.0">
-      <c t="s" s="1" r="A21">
+      <c t="s" s="2" r="A21">
         <v>56</v>
       </c>
-      <c t="s" r="C21">
+      <c t="s" s="1" r="B21">
         <v>57</v>
-      </c>
-      <c t="s" s="1" r="D21">
-        <v>58</v>
       </c>
     </row>
     <row customHeight="1" r="22" ht="18.0">
       <c t="s" s="1" r="A22">
-        <v>38</v>
-      </c>
-      <c t="s" r="B22">
+        <v>58</v>
+      </c>
+      <c t="s" r="C22">
         <v>59</v>
       </c>
       <c t="s" s="1" r="D22">
@@ -809,184 +812,195 @@
     </row>
     <row customHeight="1" r="23" ht="18.0">
       <c t="s" s="1" r="A23">
-        <v>61</v>
-      </c>
-      <c t="s" r="C23">
+        <v>40</v>
+      </c>
+      <c t="s" r="B23">
         <v>61</v>
       </c>
       <c t="s" s="1" r="D23">
         <v>62</v>
       </c>
     </row>
-    <row r="24">
+    <row customHeight="1" r="24" ht="18.0">
       <c t="s" s="1" r="A24">
         <v>63</v>
       </c>
-      <c t="s" s="1" r="C24">
+      <c t="s" r="C24">
         <v>63</v>
       </c>
       <c t="s" s="1" r="D24">
         <v>64</v>
       </c>
     </row>
-    <row customHeight="1" r="25" ht="18.0">
-      <c t="s" s="4" r="A25">
+    <row r="25">
+      <c t="s" s="1" r="A25">
         <v>65</v>
       </c>
-      <c s="1" r="C25"/>
+      <c t="s" s="1" r="C25">
+        <v>65</v>
+      </c>
+      <c t="s" s="1" r="D25">
+        <v>66</v>
+      </c>
     </row>
     <row customHeight="1" r="26" ht="18.0">
-      <c t="s" s="1" r="A26">
-        <v>66</v>
-      </c>
-      <c t="s" r="B26">
+      <c t="s" s="4" r="A26">
         <v>67</v>
       </c>
-      <c t="s" s="1" r="C26">
+      <c s="1" r="C26"/>
+    </row>
+    <row customHeight="1" r="27" ht="18.0">
+      <c t="s" s="1" r="A27">
+        <v>28</v>
+      </c>
+      <c t="s" r="B27">
         <v>68</v>
       </c>
-      <c t="s" s="1" r="D26">
+      <c t="s" s="1" r="C27">
         <v>69</v>
       </c>
-    </row>
-    <row r="27">
-      <c t="s" s="1" r="A27">
+      <c t="s" s="1" r="D27">
         <v>70</v>
-      </c>
-      <c t="s" r="B27">
-        <v>71</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
+        <v>71</v>
+      </c>
+      <c t="s" r="B28">
         <v>72</v>
-      </c>
-      <c t="s" s="1" r="C28">
-        <v>73</v>
-      </c>
-      <c t="s" s="1" r="D28">
-        <v>74</v>
       </c>
     </row>
     <row r="29">
       <c t="s" s="1" r="A29">
-        <v>18</v>
-      </c>
-      <c t="s" s="1" r="B29">
+        <v>73</v>
+      </c>
+      <c t="s" s="1" r="C29">
+        <v>74</v>
+      </c>
+      <c t="s" s="1" r="D29">
         <v>75</v>
-      </c>
-      <c t="s" s="1" r="C29">
-        <v>76</v>
-      </c>
-      <c t="s" s="1" r="D29">
-        <v>77</v>
-      </c>
-      <c t="b" r="M29">
-        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c t="s" s="1" r="A30">
+        <v>18</v>
+      </c>
+      <c t="s" s="1" r="B30">
+        <v>76</v>
+      </c>
+      <c t="s" s="1" r="C30">
+        <v>77</v>
+      </c>
+      <c t="s" s="1" r="D30">
         <v>78</v>
       </c>
+      <c t="b" r="M30">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
-      <c t="s" s="5" r="A31">
+      <c t="s" s="1" r="A31">
         <v>79</v>
       </c>
-      <c t="s" r="B31">
+    </row>
+    <row r="32">
+      <c t="s" s="5" r="A32">
         <v>80</v>
       </c>
-    </row>
-    <row r="32">
-      <c t="s" s="1" r="A32">
-        <v>70</v>
+      <c t="s" r="B32">
+        <v>81</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>6</v>
-      </c>
-      <c t="s" s="1" r="C33">
-        <v>81</v>
-      </c>
-      <c t="s" s="1" r="D33">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34">
       <c t="s" s="1" r="A34">
+        <v>6</v>
+      </c>
+      <c t="s" s="1" r="C34">
+        <v>82</v>
+      </c>
+      <c t="s" s="1" r="D34">
         <v>83</v>
-      </c>
-      <c t="s" s="1" r="C34">
-        <v>84</v>
-      </c>
-      <c t="s" s="1" r="D34">
-        <v>85</v>
       </c>
     </row>
     <row r="35">
       <c t="s" s="1" r="A35">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c t="s" s="1" r="C35">
+        <v>85</v>
+      </c>
+      <c t="s" s="1" r="D35">
         <v>86</v>
-      </c>
-      <c t="s" s="1" r="D35">
-        <v>87</v>
       </c>
     </row>
     <row r="36">
       <c t="s" s="1" r="A36">
-        <v>78</v>
+        <v>7</v>
+      </c>
+      <c t="s" s="1" r="C36">
+        <v>87</v>
+      </c>
+      <c t="s" s="1" r="D36">
+        <v>88</v>
       </c>
     </row>
     <row r="37">
-      <c t="s" s="4" r="A37">
-        <v>88</v>
-      </c>
-      <c s="1" r="D37"/>
+      <c t="s" s="1" r="A37">
+        <v>79</v>
+      </c>
     </row>
     <row r="38">
-      <c t="s" s="1" r="A38">
-        <v>35</v>
-      </c>
-      <c t="s" r="B38">
+      <c t="s" s="4" r="A38">
         <v>89</v>
       </c>
-      <c t="s" s="1" r="C38">
-        <v>90</v>
-      </c>
-      <c t="s" s="1" r="D38">
-        <v>91</v>
-      </c>
-      <c t="s" s="1" r="I38">
-        <v>92</v>
-      </c>
+      <c s="1" r="D38"/>
     </row>
     <row r="39">
       <c t="s" s="1" r="A39">
-        <v>47</v>
+        <v>37</v>
+      </c>
+      <c t="s" r="B39">
+        <v>90</v>
       </c>
       <c t="s" s="1" r="C39">
+        <v>91</v>
+      </c>
+      <c t="s" s="1" r="D39">
+        <v>92</v>
+      </c>
+      <c t="s" s="1" r="I39">
         <v>93</v>
       </c>
-      <c t="s" s="1" r="D39">
+    </row>
+    <row r="40">
+      <c t="s" s="1" r="A40">
+        <v>49</v>
+      </c>
+      <c t="s" s="1" r="C40">
         <v>94</v>
       </c>
-      <c t="s" r="E39">
+      <c t="s" s="1" r="D40">
         <v>95</v>
       </c>
-      <c r="F39">
+      <c t="s" r="E40">
+        <v>96</v>
+      </c>
+      <c r="F40">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="J39">
-        <v>96</v>
-      </c>
-      <c s="1" r="K39">
+      <c t="s" s="1" r="J40">
+        <v>97</v>
+      </c>
+      <c s="1" r="K40">
         <v>1</v>
       </c>
-      <c s="1" r="L39">
+      <c s="1" r="L40">
         <v>10</v>
       </c>
     </row>
@@ -1010,15 +1024,15 @@
         <v>2</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1038,7 +1052,7 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c t="s" s="1" r="B1">
         <v>2</v>
@@ -1049,101 +1063,101 @@
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c t="s" s="1" r="B6">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c t="s" s="1" r="B9">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12">
@@ -1162,10 +1176,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B13">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c t="s" r="C13">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14">
@@ -1173,10 +1187,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B14">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c t="s" r="C14">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15">
@@ -1184,10 +1198,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B15">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" r="C15">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16">
@@ -1195,10 +1209,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B16">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c t="s" r="C16">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17">
@@ -1206,10 +1220,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B17">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c t="s" r="C17">
-        <v>66</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18">
@@ -1217,10 +1231,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B18">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c t="s" r="C18">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19">
@@ -1228,10 +1242,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B19">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c t="s" r="C19">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20">
@@ -1239,10 +1253,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B20">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c t="s" r="C20">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1261,23 +1275,23 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c s="1" r="B3">
         <v>1</v>
@@ -1285,10 +1299,10 @@
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding prompt link example
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="143">
   <si>
     <t>type</t>
   </si>
@@ -291,6 +291,30 @@
     <t>label media_end</t>
   </si>
   <si>
+    <t>selected(data('examples'), 'prompt_link')</t>
+  </si>
+  <si>
+    <t>&lt;a href="{{promptLink "unreachable"}}"&gt;This is a link to another prompt&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>label prompt_link_return</t>
+  </si>
+  <si>
+    <t>goto unreachable_end</t>
+  </si>
+  <si>
+    <t>unreachable</t>
+  </si>
+  <si>
+    <t>This prompt is unreachable except by links.</t>
+  </si>
+  <si>
+    <t>goto prompt_link_return</t>
+  </si>
+  <si>
+    <t>label unreachable_end</t>
+  </si>
+  <si>
     <t>selected(data('examples'), 'custom_template')</t>
   </si>
   <si>
@@ -397,6 +421,12 @@
   </si>
   <si>
     <t>custom template</t>
+  </si>
+  <si>
+    <t>prompt_link</t>
+  </si>
+  <si>
+    <t>prompt linking</t>
   </si>
   <si>
     <t>setting</t>
@@ -563,7 +593,7 @@
       <c t="s" s="1" r="C1">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c t="s" s="3" r="D1">
         <v>3</v>
       </c>
       <c t="s" s="1" r="E1">
@@ -712,7 +742,7 @@
       <c t="s" s="1" r="C14">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="D14">
+      <c t="s" s="3" r="D14">
         <v>38</v>
       </c>
       <c t="s" s="1" r="E14">
@@ -723,7 +753,7 @@
       <c t="s" s="1" r="A15">
         <v>40</v>
       </c>
-      <c t="s" s="1" r="D15">
+      <c t="s" s="3" r="D15">
         <v>41</v>
       </c>
       <c t="s" r="E15">
@@ -806,7 +836,7 @@
       <c t="s" r="C22">
         <v>59</v>
       </c>
-      <c t="s" s="1" r="D22">
+      <c t="s" s="3" r="D22">
         <v>60</v>
       </c>
     </row>
@@ -817,7 +847,7 @@
       <c t="s" r="B23">
         <v>61</v>
       </c>
-      <c t="s" s="1" r="D23">
+      <c t="s" s="3" r="D23">
         <v>62</v>
       </c>
     </row>
@@ -828,7 +858,7 @@
       <c t="s" r="C24">
         <v>63</v>
       </c>
-      <c t="s" s="1" r="D24">
+      <c t="s" s="3" r="D24">
         <v>64</v>
       </c>
     </row>
@@ -839,7 +869,7 @@
       <c t="s" s="1" r="C25">
         <v>65</v>
       </c>
-      <c t="s" s="1" r="D25">
+      <c t="s" s="3" r="D25">
         <v>66</v>
       </c>
     </row>
@@ -859,7 +889,7 @@
       <c t="s" s="1" r="C27">
         <v>69</v>
       </c>
-      <c t="s" s="1" r="D27">
+      <c t="s" s="3" r="D27">
         <v>70</v>
       </c>
     </row>
@@ -878,7 +908,7 @@
       <c t="s" s="1" r="C29">
         <v>74</v>
       </c>
-      <c t="s" s="1" r="D29">
+      <c t="s" s="3" r="D29">
         <v>75</v>
       </c>
     </row>
@@ -892,7 +922,7 @@
       <c t="s" s="1" r="C30">
         <v>77</v>
       </c>
-      <c t="s" s="1" r="D30">
+      <c t="s" s="3" r="D30">
         <v>78</v>
       </c>
       <c t="b" r="M30">
@@ -924,7 +954,7 @@
       <c t="s" s="1" r="C34">
         <v>82</v>
       </c>
-      <c t="s" s="1" r="D34">
+      <c t="s" s="3" r="D34">
         <v>83</v>
       </c>
     </row>
@@ -935,7 +965,7 @@
       <c t="s" s="1" r="C35">
         <v>85</v>
       </c>
-      <c t="s" s="1" r="D35">
+      <c t="s" s="3" r="D35">
         <v>86</v>
       </c>
     </row>
@@ -946,7 +976,7 @@
       <c t="s" s="1" r="C36">
         <v>87</v>
       </c>
-      <c t="s" s="1" r="D36">
+      <c t="s" s="3" r="D36">
         <v>88</v>
       </c>
     </row>
@@ -959,48 +989,94 @@
       <c t="s" s="4" r="A38">
         <v>89</v>
       </c>
-      <c s="1" r="D38"/>
+      <c s="3" r="D38"/>
     </row>
     <row r="39">
       <c t="s" s="1" r="A39">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c t="s" r="B39">
         <v>90</v>
       </c>
-      <c t="s" s="1" r="C39">
+      <c t="s" s="3" r="D39">
         <v>91</v>
       </c>
-      <c t="s" s="1" r="D39">
+    </row>
+    <row r="40">
+      <c t="s" s="4" r="A40">
         <v>92</v>
       </c>
-      <c t="s" s="1" r="I39">
+      <c s="3" r="D40"/>
+    </row>
+    <row r="41">
+      <c t="s" s="5" r="A41">
         <v>93</v>
       </c>
-    </row>
-    <row r="40">
-      <c t="s" s="1" r="A40">
+      <c s="3" r="D41"/>
+    </row>
+    <row r="42">
+      <c t="s" s="1" r="A42">
+        <v>40</v>
+      </c>
+      <c t="s" r="C42">
+        <v>94</v>
+      </c>
+      <c t="s" s="3" r="D42">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43">
+      <c t="s" s="5" r="A43">
+        <v>96</v>
+      </c>
+      <c s="3" r="D43"/>
+    </row>
+    <row r="44">
+      <c t="s" s="4" r="A44">
+        <v>97</v>
+      </c>
+      <c s="3" r="D44"/>
+    </row>
+    <row r="45">
+      <c t="s" s="1" r="A45">
+        <v>37</v>
+      </c>
+      <c t="s" r="B45">
+        <v>98</v>
+      </c>
+      <c t="s" s="1" r="C45">
+        <v>99</v>
+      </c>
+      <c t="s" s="3" r="D45">
+        <v>100</v>
+      </c>
+      <c t="s" s="1" r="I45">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46">
+      <c t="s" s="1" r="A46">
         <v>49</v>
       </c>
-      <c t="s" s="1" r="C40">
-        <v>94</v>
-      </c>
-      <c t="s" s="1" r="D40">
-        <v>95</v>
-      </c>
-      <c t="s" r="E40">
-        <v>96</v>
-      </c>
-      <c r="F40">
+      <c t="s" s="1" r="C46">
+        <v>102</v>
+      </c>
+      <c t="s" s="3" r="D46">
+        <v>103</v>
+      </c>
+      <c t="s" r="E46">
+        <v>104</v>
+      </c>
+      <c r="F46">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="J40">
-        <v>97</v>
-      </c>
-      <c s="1" r="K40">
+      <c t="s" s="1" r="J46">
+        <v>105</v>
+      </c>
+      <c s="1" r="K46">
         <v>1</v>
       </c>
-      <c s="1" r="L40">
+      <c s="1" r="L46">
         <v>10</v>
       </c>
     </row>
@@ -1024,15 +1100,15 @@
         <v>2</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1052,7 +1128,7 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="B1">
         <v>2</v>
@@ -1063,101 +1139,101 @@
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="B6">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="B9">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12">
@@ -1176,10 +1252,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B13">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c t="s" r="C13">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14">
@@ -1187,10 +1263,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B14">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c t="s" r="C14">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15">
@@ -1198,10 +1274,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B15">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c t="s" r="C15">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16">
@@ -1231,10 +1307,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B18">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c t="s" r="C18">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19">
@@ -1242,10 +1318,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B19">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c t="s" r="C19">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20">
@@ -1253,10 +1329,21 @@
         <v>14</v>
       </c>
       <c t="s" r="B20">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c t="s" r="C20">
-        <v>125</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21">
+      <c t="s" r="A21">
+        <v>14</v>
+      </c>
+      <c t="s" r="B21">
+        <v>134</v>
+      </c>
+      <c t="s" r="C21">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1275,23 +1362,23 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c s="1" r="B3">
         <v>1</v>
@@ -1299,10 +1386,10 @@
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding support for jQm themes and a theme setting
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="147">
   <si>
     <t>type</t>
   </si>
@@ -448,6 +448,18 @@
   </si>
   <si>
     <t>Example Form</t>
+  </si>
+  <si>
+    <t>font-size</t>
+  </si>
+  <si>
+    <t>11pt</t>
+  </si>
+  <si>
+    <t>theme</t>
+  </si>
+  <si>
+    <t>square</t>
   </si>
 </sst>
 </file>
@@ -1392,6 +1404,22 @@
         <v>142</v>
       </c>
     </row>
+    <row r="5">
+      <c t="s" r="A5">
+        <v>143</v>
+      </c>
+      <c t="s" r="B5">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6">
+      <c t="s" r="A6">
+        <v>145</v>
+      </c>
+      <c t="s" r="B6">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactoring custom appearance demo into a separate form.
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="144">
   <si>
     <t>type</t>
   </si>
@@ -127,44 +127,46 @@
     <t>not(selected(data('examples'), 'label_features'))</t>
   </si>
   <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>&lt;u&gt;Labels&lt;/u&gt; &lt;i&gt;can&lt;/i&gt; contain &lt;span style="color:red;"&gt;HTML&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>So can &lt;b&gt;hints&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Labels can contain &amp;lt;img&amp;gt; and &amp;lt;audio&amp;gt; HTML tags, but it is often easier to add media via the image and audio columns.</t>
+  </si>
+  <si>
+    <t>audio/carrioncrow.mp3</t>
+  </si>
+  <si>
+    <t>img/dolphin.png</t>
+  </si>
+  <si>
     <t>text</t>
   </si>
   <si>
     <t>Enter your name</t>
   </si>
   <si>
-    <t>Please use your full name</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>{{#if name}}
+    <t>It will be used in the next question.</t>
+  </si>
+  <si>
+    <t>&lt;h3&gt;
+This label uses Handlesbars template features:
+&lt;/h3&gt;
+{{#if name}}
 Hello {{name}}!
 {{else}}
 Name not entered.
-{{/if}}
-This label is a handlesbars template.</t>
+{{/if}}</t>
   </si>
   <si>
     <t>Handlebars templates allow labels to change depending on the values previously entered.</t>
   </si>
   <si>
-    <t>&lt;u&gt;Labels&lt;/u&gt; &lt;i&gt;can&lt;/i&gt; contain &lt;span style="color:red;"&gt;HTML&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>So can &lt;b&gt;hints&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>Labels can contain &amp;lt;img&amp;gt; and &amp;lt;audio&amp;gt; HTML tags, but it is often easier to add media via the image and audio columns.</t>
-  </si>
-  <si>
-    <t>audio/carrioncrow.mp3</t>
-  </si>
-  <si>
-    <t>img/dolphin.png</t>
-  </si>
-  <si>
     <t>label label_features_end</t>
   </si>
   <si>
@@ -204,16 +206,19 @@
     <t>When were you born?</t>
   </si>
   <si>
-    <t>data('born').getDay() === now().getDay() &amp;&amp; data('born').getMonth() === now().getMonth()</t>
+    <t>data('born') &amp;&amp; data('born').getDay() === now().getDay() &amp;&amp; data('born').getMonth() === now().getMonth()</t>
   </si>
   <si>
     <t>Happy Birthday!</t>
   </si>
   <si>
+    <t>This prompt shows how to use dates in fomulas.</t>
+  </si>
+  <si>
     <t>time</t>
   </si>
   <si>
-    <t>What time is it?</t>
+    <t>What time do you usually wake up?</t>
   </si>
   <si>
     <t>datetime</t>
@@ -448,18 +453,6 @@
   </si>
   <si>
     <t>Example Form</t>
-  </si>
-  <si>
-    <t>font-size</t>
-  </si>
-  <si>
-    <t>11pt</t>
-  </si>
-  <si>
-    <t>theme</t>
-  </si>
-  <si>
-    <t>square</t>
   </si>
 </sst>
 </file>
@@ -751,49 +744,49 @@
       <c t="s" s="1" r="A14">
         <v>37</v>
       </c>
-      <c t="s" s="1" r="C14">
-        <v>2</v>
-      </c>
-      <c t="s" s="3" r="D14">
+      <c t="s" r="D14">
         <v>38</v>
       </c>
-      <c t="s" s="1" r="E14">
+      <c t="s" r="E14">
         <v>39</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
+        <v>37</v>
+      </c>
+      <c t="s" s="3" r="D15">
         <v>40</v>
       </c>
-      <c t="s" s="3" r="D15">
+      <c t="s" s="1" r="G15">
         <v>41</v>
       </c>
-      <c t="s" r="E15">
+      <c t="s" s="1" r="H15">
         <v>42</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>40</v>
-      </c>
-      <c t="s" r="D16">
         <v>43</v>
       </c>
-      <c t="s" r="E16">
+      <c t="s" s="1" r="C16">
+        <v>2</v>
+      </c>
+      <c t="s" s="3" r="D16">
         <v>44</v>
+      </c>
+      <c t="s" s="1" r="E16">
+        <v>45</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c t="s" s="3" r="D17">
-        <v>45</v>
-      </c>
-      <c t="s" s="1" r="G17">
         <v>46</v>
       </c>
-      <c t="s" s="1" r="H17">
+      <c t="s" r="E17">
         <v>47</v>
       </c>
     </row>
@@ -854,7 +847,7 @@
     </row>
     <row customHeight="1" r="23" ht="18.0">
       <c t="s" s="1" r="A23">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c t="s" r="B23">
         <v>61</v>
@@ -862,32 +855,35 @@
       <c t="s" s="3" r="D23">
         <v>62</v>
       </c>
+      <c t="s" r="E23">
+        <v>63</v>
+      </c>
     </row>
     <row customHeight="1" r="24" ht="18.0">
       <c t="s" s="1" r="A24">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c t="s" r="C24">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c t="s" s="3" r="D24">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25">
       <c t="s" s="1" r="A25">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c t="s" s="1" r="C25">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c t="s" s="3" r="D25">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row customHeight="1" r="26" ht="18.0">
       <c t="s" s="4" r="A26">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c s="1" r="C26"/>
     </row>
@@ -896,32 +892,32 @@
         <v>28</v>
       </c>
       <c t="s" r="B27">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c t="s" s="1" r="C27">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c t="s" s="3" r="D27">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c t="s" r="B28">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29">
       <c t="s" s="1" r="A29">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c t="s" s="1" r="C29">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c t="s" s="3" r="D29">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30">
@@ -929,13 +925,13 @@
         <v>18</v>
       </c>
       <c t="s" s="1" r="B30">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="C30">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c t="s" s="3" r="D30">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c t="b" r="M30">
         <v>1</v>
@@ -943,20 +939,20 @@
     </row>
     <row r="31">
       <c t="s" s="1" r="A31">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32">
       <c t="s" s="5" r="A32">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c t="s" r="B32">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34">
@@ -964,21 +960,21 @@
         <v>6</v>
       </c>
       <c t="s" s="1" r="C34">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c t="s" s="3" r="D34">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35">
       <c t="s" s="1" r="A35">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c t="s" s="1" r="C35">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c t="s" s="3" r="D35">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36">
@@ -986,84 +982,84 @@
         <v>7</v>
       </c>
       <c t="s" s="1" r="C36">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c t="s" s="3" r="D36">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37">
       <c t="s" s="1" r="A37">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38">
       <c t="s" s="4" r="A38">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c s="3" r="D38"/>
     </row>
     <row r="39">
       <c t="s" s="1" r="A39">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c t="s" r="B39">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c t="s" s="3" r="D39">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40">
       <c t="s" s="4" r="A40">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c s="3" r="D40"/>
     </row>
     <row r="41">
       <c t="s" s="5" r="A41">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c s="3" r="D41"/>
     </row>
     <row r="42">
       <c t="s" s="1" r="A42">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c t="s" r="C42">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c t="s" s="3" r="D42">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43">
       <c t="s" s="5" r="A43">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c s="3" r="D43"/>
     </row>
     <row r="44">
       <c t="s" s="4" r="A44">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c s="3" r="D44"/>
     </row>
     <row r="45">
       <c t="s" s="1" r="A45">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c t="s" r="B45">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c t="s" s="1" r="C45">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c t="s" s="3" r="D45">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c t="s" s="1" r="I45">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46">
@@ -1071,19 +1067,19 @@
         <v>49</v>
       </c>
       <c t="s" s="1" r="C46">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c t="s" s="3" r="D46">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c t="s" r="E46">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F46">
         <v>5</v>
       </c>
       <c t="s" s="1" r="J46">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c s="1" r="K46">
         <v>1</v>
@@ -1112,15 +1108,15 @@
         <v>2</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1140,7 +1136,7 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c t="s" s="1" r="B1">
         <v>2</v>
@@ -1151,101 +1147,101 @@
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B6">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B9">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12">
@@ -1264,10 +1260,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B13">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c t="s" r="C13">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14">
@@ -1275,10 +1271,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B14">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c t="s" r="C14">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15">
@@ -1286,10 +1282,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B15">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c t="s" r="C15">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16">
@@ -1297,10 +1293,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B16">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c t="s" r="C16">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17">
@@ -1319,10 +1315,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B18">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c t="s" r="C18">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19">
@@ -1330,10 +1326,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B19">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c t="s" r="C19">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20">
@@ -1341,10 +1337,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B20">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c t="s" r="C20">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21">
@@ -1352,10 +1348,10 @@
         <v>14</v>
       </c>
       <c t="s" r="B21">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c t="s" r="C21">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1374,23 +1370,23 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c s="1" r="B3">
         <v>1</v>
@@ -1398,26 +1394,10 @@
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5">
-      <c t="s" r="A5">
         <v>143</v>
-      </c>
-      <c t="s" r="B5">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" r="A6">
-        <v>145</v>
-      </c>
-      <c t="s" r="B6">
-        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Making the screen flash white to provide swipe feedback and adding weight for age plot.
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="153">
   <si>
     <t>type</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>inputAttributes.max</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>constraint_message</t>
   </si>
   <si>
     <t>required</t>
@@ -323,13 +329,34 @@
     <t>selected(data('examples'), 'custom_template')</t>
   </si>
   <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Enter age:</t>
+  </si>
+  <si>
+    <t>data('age') &lt;= 20</t>
+  </si>
+  <si>
+    <t>The grown chart only has data for below 20 years. This age you entered will not fit on the plot.</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>Enter weight:</t>
+  </si>
+  <si>
     <t>specialTemplateTest</t>
   </si>
   <si>
-    <t>This is a custom template that uses D3.js:</t>
-  </si>
-  <si>
-    <t>test.handlebars</t>
+    <t>This is a custom template that uses D3.js to plot an age and weight on a growth chart:</t>
+  </si>
+  <si>
+    <t>ageWeightPlot.handlebars</t>
   </si>
   <si>
     <t>rating</t>
@@ -585,7 +612,7 @@
     <col min="10" customWidth="1" max="10" width="18.29"/>
     <col min="11" customWidth="1" max="11" width="18.43"/>
     <col min="12" customWidth="1" max="12" width="19.0"/>
-    <col min="13" customWidth="1" max="13" width="27.0"/>
+    <col min="15" customWidth="1" max="15" width="27.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -628,81 +655,87 @@
       <c t="s" s="1" r="M1">
         <v>12</v>
       </c>
+      <c t="s" s="1" r="N1">
+        <v>13</v>
+      </c>
+      <c t="s" s="1" r="O1">
+        <v>14</v>
+      </c>
     </row>
     <row customHeight="1" r="2" ht="18.0">
       <c t="s" s="1" r="A2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c t="s" r="C2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="s" r="D2">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="2" r="A3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c t="s" r="C4">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c t="s" r="D4">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c t="s" r="E4">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c t="s" r="A5">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c t="s" r="B5">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="4" r="A6">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="2" r="A7">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c t="s" r="A8">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c t="s" r="C8">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c t="s" r="D8">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
       <c t="s" r="A9">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c t="s" r="C9">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c t="s" r="D9">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
@@ -710,10 +743,10 @@
         <v>7</v>
       </c>
       <c t="s" r="C10">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c t="s" r="D10">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
@@ -721,238 +754,238 @@
         <v>6</v>
       </c>
       <c t="s" r="C11">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c t="s" r="D11">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
       <c t="s" s="4" r="A12">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13">
       <c t="s" s="2" r="A13">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c t="s" s="1" r="B13">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c t="s" r="D14">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c t="s" r="E14">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c t="s" s="3" r="D15">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c t="s" s="1" r="G15">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c t="s" s="1" r="H15">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16">
       <c t="s" s="1" r="A16">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c t="s" s="1" r="C16">
         <v>2</v>
       </c>
       <c t="s" s="3" r="D16">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c t="s" s="1" r="E16">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c t="s" s="3" r="D17">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c t="s" r="E17">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row customHeight="1" r="18" ht="18.0">
       <c t="s" s="4" r="A18">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c t="s" r="B19">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c t="s" r="C19">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c t="s" r="D19">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20">
       <c t="s" s="1" r="A20">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c t="s" r="B20">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c t="s" r="C20">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c t="s" r="D20">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c t="s" r="F20">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row customHeight="1" r="21" ht="18.0">
       <c t="s" s="2" r="A21">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c t="s" s="1" r="B21">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row customHeight="1" r="22" ht="18.0">
       <c t="s" s="1" r="A22">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c t="s" r="C22">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c t="s" s="3" r="D22">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row customHeight="1" r="23" ht="18.0">
       <c t="s" s="1" r="A23">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c t="s" r="B23">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c t="s" s="3" r="D23">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c t="s" r="E23">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row customHeight="1" r="24" ht="18.0">
       <c t="s" s="1" r="A24">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c t="s" r="C24">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c t="s" s="3" r="D24">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25">
       <c t="s" s="1" r="A25">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c t="s" s="1" r="C25">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c t="s" s="3" r="D25">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row customHeight="1" r="26" ht="18.0">
       <c t="s" s="4" r="A26">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c s="1" r="C26"/>
     </row>
     <row customHeight="1" r="27" ht="18.0">
       <c t="s" s="1" r="A27">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c t="s" r="B27">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c t="s" s="1" r="C27">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c t="s" s="3" r="D27">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c t="s" r="B28">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29">
       <c t="s" s="1" r="A29">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c t="s" s="1" r="C29">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c t="s" s="3" r="D29">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30">
       <c t="s" s="1" r="A30">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c t="s" s="1" r="B30">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c t="s" s="1" r="C30">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c t="s" s="3" r="D30">
-        <v>79</v>
-      </c>
-      <c t="b" r="M30">
+        <v>81</v>
+      </c>
+      <c t="b" r="O30">
         <v>1</v>
       </c>
     </row>
     <row r="31">
       <c t="s" s="1" r="A31">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32">
       <c t="s" s="5" r="A32">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c t="s" r="B32">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34">
@@ -960,21 +993,21 @@
         <v>6</v>
       </c>
       <c t="s" s="1" r="C34">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c t="s" s="3" r="D34">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35">
       <c t="s" s="1" r="A35">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c t="s" s="1" r="C35">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c t="s" s="3" r="D35">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36">
@@ -982,109 +1015,152 @@
         <v>7</v>
       </c>
       <c t="s" s="1" r="C36">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c t="s" s="3" r="D36">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37">
       <c t="s" s="1" r="A37">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38">
       <c t="s" s="4" r="A38">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c s="3" r="D38"/>
     </row>
     <row r="39">
       <c t="s" s="1" r="A39">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c t="s" r="B39">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c t="s" s="3" r="D39">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40">
       <c t="s" s="4" r="A40">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c s="3" r="D40"/>
     </row>
     <row r="41">
       <c t="s" s="5" r="A41">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c s="3" r="D41"/>
     </row>
     <row r="42">
       <c t="s" s="1" r="A42">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c t="s" r="C42">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c t="s" s="3" r="D42">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43">
       <c t="s" s="5" r="A43">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c s="3" r="D43"/>
     </row>
     <row r="44">
       <c t="s" s="4" r="A44">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c s="3" r="D44"/>
     </row>
     <row r="45">
       <c t="s" s="1" r="A45">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c t="s" r="B45">
-        <v>99</v>
-      </c>
-      <c t="s" s="1" r="C45">
-        <v>100</v>
-      </c>
-      <c t="s" s="3" r="D45">
         <v>101</v>
       </c>
-      <c t="s" s="1" r="I45">
-        <v>102</v>
-      </c>
+      <c s="3" r="D45"/>
     </row>
     <row r="46">
       <c t="s" s="1" r="A46">
-        <v>49</v>
-      </c>
-      <c t="s" s="1" r="C46">
+        <v>51</v>
+      </c>
+      <c t="s" r="C46">
+        <v>102</v>
+      </c>
+      <c t="s" s="3" r="D46">
         <v>103</v>
       </c>
-      <c t="s" s="3" r="D46">
+      <c t="s" r="M46">
         <v>104</v>
       </c>
-      <c t="s" r="E46">
+      <c t="s" r="N46">
         <v>105</v>
       </c>
-      <c r="F46">
+    </row>
+    <row r="47">
+      <c t="s" s="1" r="A47">
+        <v>106</v>
+      </c>
+      <c t="s" r="C47">
+        <v>107</v>
+      </c>
+      <c t="s" s="3" r="D47">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48">
+      <c t="s" s="1" r="A48">
+        <v>82</v>
+      </c>
+      <c s="3" r="D48"/>
+    </row>
+    <row r="49">
+      <c t="s" s="1" r="A49">
+        <v>39</v>
+      </c>
+      <c t="s" r="B49">
+        <v>101</v>
+      </c>
+      <c t="s" s="1" r="C49">
+        <v>109</v>
+      </c>
+      <c t="s" s="3" r="D49">
+        <v>110</v>
+      </c>
+      <c t="s" s="1" r="I49">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50">
+      <c t="s" s="1" r="A50">
+        <v>51</v>
+      </c>
+      <c t="s" s="1" r="C50">
+        <v>112</v>
+      </c>
+      <c t="s" s="3" r="D50">
+        <v>113</v>
+      </c>
+      <c t="s" r="E50">
+        <v>114</v>
+      </c>
+      <c r="F50">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="J46">
-        <v>106</v>
-      </c>
-      <c s="1" r="K46">
+      <c t="s" s="1" r="J50">
+        <v>115</v>
+      </c>
+      <c s="1" r="K50">
         <v>1</v>
       </c>
-      <c s="1" r="L46">
+      <c s="1" r="L50">
         <v>10</v>
       </c>
     </row>
@@ -1108,15 +1184,15 @@
         <v>2</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1136,7 +1212,7 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c t="s" s="1" r="B1">
         <v>2</v>
@@ -1147,211 +1223,211 @@
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c t="s" s="1" r="B6">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c t="s" s="1" r="B9">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12">
       <c t="s" r="A12">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="s" r="B12">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c t="s" r="C12">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
       <c t="s" r="A13">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="s" r="B13">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c t="s" r="C13">
-        <v>125</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14">
       <c t="s" r="A14">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="s" r="B14">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c t="s" r="C14">
-        <v>127</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15">
       <c t="s" r="A15">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="s" r="B15">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c t="s" r="C15">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16">
       <c t="s" r="A16">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="s" r="B16">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c t="s" r="C16">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17">
       <c t="s" r="A17">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="s" r="B17">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c t="s" r="C17">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18">
       <c t="s" r="A18">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="s" r="B18">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c t="s" r="C18">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19">
       <c t="s" r="A19">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="s" r="B19">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c t="s" r="C19">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20">
       <c t="s" r="A20">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="s" r="B20">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c t="s" r="C20">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21">
       <c t="s" r="A21">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="s" r="B21">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c t="s" r="C21">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1370,23 +1446,23 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>140</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c s="1" r="B3">
         <v>1</v>
@@ -1394,10 +1470,10 @@
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding sex selection to weight for age plot example.
</commit_message>
<xml_diff>
--- a/form-files/example/example.xlsx
+++ b/form-files/example/example.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="161">
   <si>
     <t>type</t>
   </si>
@@ -329,10 +329,16 @@
     <t>selected(data('examples'), 'custom_template')</t>
   </si>
   <si>
+    <t>The following data will be used to generate a weight for age plot.</t>
+  </si>
+  <si>
     <t>age</t>
   </si>
   <si>
-    <t>Enter age:</t>
+    <t>Enter age (in years):</t>
+  </si>
+  <si>
+    <t>Must be less than 20.</t>
   </si>
   <si>
     <t>data('age') &lt;= 20</t>
@@ -347,7 +353,16 @@
     <t>weight</t>
   </si>
   <si>
-    <t>Enter weight:</t>
+    <t>Enter weight (in lbs):</t>
+  </si>
+  <si>
+    <t>select_one sexes</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>Enter sex:</t>
   </si>
   <si>
     <t>specialTemplateTest</t>
@@ -459,6 +474,15 @@
   </si>
   <si>
     <t>prompt linking</t>
+  </si>
+  <si>
+    <t>sexes</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
   <si>
     <t>setting</t>
@@ -1089,78 +1113,100 @@
     </row>
     <row r="46">
       <c t="s" s="1" r="A46">
-        <v>51</v>
-      </c>
-      <c t="s" r="C46">
+        <v>39</v>
+      </c>
+      <c t="s" s="3" r="D46">
         <v>102</v>
-      </c>
-      <c t="s" s="3" r="D46">
-        <v>103</v>
-      </c>
-      <c t="s" r="M46">
-        <v>104</v>
-      </c>
-      <c t="s" r="N46">
-        <v>105</v>
       </c>
     </row>
     <row r="47">
       <c t="s" s="1" r="A47">
+        <v>51</v>
+      </c>
+      <c t="s" r="C47">
+        <v>103</v>
+      </c>
+      <c t="s" s="3" r="D47">
+        <v>104</v>
+      </c>
+      <c t="s" r="E47">
+        <v>105</v>
+      </c>
+      <c t="s" r="M47">
         <v>106</v>
       </c>
-      <c t="s" r="C47">
+      <c t="s" r="N47">
         <v>107</v>
-      </c>
-      <c t="s" s="3" r="D47">
-        <v>108</v>
       </c>
     </row>
     <row r="48">
       <c t="s" s="1" r="A48">
-        <v>82</v>
-      </c>
-      <c s="3" r="D48"/>
+        <v>108</v>
+      </c>
+      <c t="s" r="C48">
+        <v>109</v>
+      </c>
+      <c t="s" s="3" r="D48">
+        <v>110</v>
+      </c>
     </row>
     <row r="49">
       <c t="s" s="1" r="A49">
-        <v>39</v>
-      </c>
-      <c t="s" r="B49">
-        <v>101</v>
-      </c>
-      <c t="s" s="1" r="C49">
-        <v>109</v>
+        <v>111</v>
+      </c>
+      <c t="s" r="C49">
+        <v>112</v>
       </c>
       <c t="s" s="3" r="D49">
-        <v>110</v>
-      </c>
-      <c t="s" s="1" r="I49">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50">
       <c t="s" s="1" r="A50">
+        <v>82</v>
+      </c>
+      <c s="3" r="D50"/>
+    </row>
+    <row r="51">
+      <c t="s" s="1" r="A51">
+        <v>39</v>
+      </c>
+      <c t="s" r="B51">
+        <v>101</v>
+      </c>
+      <c t="s" s="1" r="C51">
+        <v>114</v>
+      </c>
+      <c t="s" s="3" r="D51">
+        <v>115</v>
+      </c>
+      <c t="s" s="1" r="I51">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52">
+      <c t="s" s="1" r="A52">
         <v>51</v>
       </c>
-      <c t="s" s="1" r="C50">
-        <v>112</v>
-      </c>
-      <c t="s" s="3" r="D50">
-        <v>113</v>
-      </c>
-      <c t="s" r="E50">
-        <v>114</v>
-      </c>
-      <c r="F50">
+      <c t="s" s="1" r="C52">
+        <v>117</v>
+      </c>
+      <c t="s" s="3" r="D52">
+        <v>118</v>
+      </c>
+      <c t="s" r="E52">
+        <v>119</v>
+      </c>
+      <c r="F52">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="J50">
-        <v>115</v>
-      </c>
-      <c s="1" r="K50">
+      <c t="s" s="1" r="J52">
+        <v>120</v>
+      </c>
+      <c s="1" r="K52">
         <v>1</v>
       </c>
-      <c s="1" r="L50">
+      <c s="1" r="L52">
         <v>10</v>
       </c>
     </row>
@@ -1184,15 +1230,15 @@
         <v>2</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1212,7 +1258,7 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c t="s" s="1" r="B1">
         <v>2</v>
@@ -1223,101 +1269,101 @@
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c t="s" s="1" r="B3">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5">
       <c t="s" s="1" r="A5">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c t="s" s="1" r="B5">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6">
       <c t="s" s="1" r="A6">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c t="s" s="1" r="B6">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7">
       <c t="s" s="1" r="A7">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c t="s" s="1" r="B7">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8">
       <c t="s" s="1" r="A8">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c t="s" s="1" r="B8">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c t="s" s="1" r="B9">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c t="s" s="1" r="B10">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12">
@@ -1336,10 +1382,10 @@
         <v>16</v>
       </c>
       <c t="s" r="B13">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c t="s" r="C13">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14">
@@ -1347,10 +1393,10 @@
         <v>16</v>
       </c>
       <c t="s" r="B14">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c t="s" r="C14">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15">
@@ -1358,10 +1404,10 @@
         <v>16</v>
       </c>
       <c t="s" r="B15">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c t="s" r="C15">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16">
@@ -1391,10 +1437,10 @@
         <v>16</v>
       </c>
       <c t="s" r="B18">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c t="s" r="C18">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19">
@@ -1402,10 +1448,10 @@
         <v>16</v>
       </c>
       <c t="s" r="B19">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c t="s" r="C19">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20">
@@ -1413,10 +1459,10 @@
         <v>16</v>
       </c>
       <c t="s" r="B20">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c t="s" r="C20">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21">
@@ -1424,10 +1470,32 @@
         <v>16</v>
       </c>
       <c t="s" r="B21">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c t="s" r="C21">
-        <v>145</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23">
+      <c t="s" r="A23">
+        <v>151</v>
+      </c>
+      <c t="s" r="B23">
+        <v>152</v>
+      </c>
+      <c t="s" r="C23">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24">
+      <c t="s" r="A24">
+        <v>151</v>
+      </c>
+      <c t="s" r="B24">
+        <v>153</v>
+      </c>
+      <c t="s" r="C24">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1446,23 +1514,23 @@
   <sheetData>
     <row r="1">
       <c t="s" s="1" r="A1">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2">
       <c t="s" s="1" r="A2">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3">
       <c t="s" s="1" r="A3">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c s="1" r="B3">
         <v>1</v>
@@ -1470,10 +1538,10 @@
     </row>
     <row r="4">
       <c t="s" s="1" r="A4">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c t="s" s="1" r="B4">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>